<commit_message>
new construction logic developed and verified
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Parameter_Building_Coverage.xlsx
+++ b/projects/test_building/input/Parameter_Building_Coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/test_building/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9486372D-C4C6-F844-9F51-0DFEA08C7DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A980374-2DCC-694B-B7F4-E64243ED034B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-420" yWindow="-20780" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38280" yWindow="-19580" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
@@ -399,7 +399,7 @@
   <dimension ref="A1:C402"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
input tables are checked and extended to 2010. All values from 2010 to 2020 (at least) are filled in, so the model take any year from 2010 to 2020 as base year.
For Scenario_Building.xlsx, for 2010 column where id_building_construction_period = 13, values are revised to 0. But, in some other tables which has the column id_building_construction_period, it might not be consistent (not big problem either):

Scenario_Building_UnitArea.xlsx
Scenario_Radiator.xlsx
Scenario_HeatingTechnology_Main.xlsx
Scenario_BuildingComponent_Option.xlsx
Scenario_Building_ConstructionPeriod.xlsx
Parameter_Building_ConstructionYear.xlsx
Scenario_HeatingTechnology_Second.xlsx
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Parameter_Building_Coverage.xlsx
+++ b/projects/test_building/input/Parameter_Building_Coverage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/test_building/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A980374-2DCC-694B-B7F4-E64243ED034B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBC40D6-B65D-674A-BDA9-2B3DE1A8E9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38280" yWindow="-19580" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,7 +427,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
data collector updated: (1) building stock is collected and saved each year, (2) old code on (historical) renovation rate removed
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Parameter_Building_Coverage.xlsx
+++ b/projects/test_building/input/Parameter_Building_Coverage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/test_building/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBC40D6-B65D-674A-BDA9-2B3DE1A8E9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8205116C-BFE7-374F-B293-FB8872AFE1EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38280" yWindow="-19580" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,7 +427,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>1E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
scenario dependent tables revised: building component and heating technology availability
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Parameter_Building_Coverage.xlsx
+++ b/projects/test_building/input/Parameter_Building_Coverage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/test_building/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF7DE97-0861-3D46-A9E1-051D477DE500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80936421-70D9-B141-A587-51FB79600E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38280" yWindow="-19580" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,13 +399,12 @@
   <dimension ref="A1:C402"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -427,7 +426,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated hot water intensity for calibration
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Parameter_Building_Coverage.xlsx
+++ b/projects/test_building/input/Parameter_Building_Coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/test_building/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CF3F9F-4EAF-6841-8B4F-D7A839F999AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A1DC63-833F-9648-92A4-B1F9ADB476BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35560" yWindow="-20520" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
@@ -399,7 +399,7 @@
   <dimension ref="A1:C402"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -426,7 +426,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -437,7 +437,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -448,7 +448,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -459,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -470,7 +470,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -481,7 +481,7 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -492,7 +492,7 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -503,7 +503,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -514,7 +514,7 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -525,7 +525,7 @@
         <v>3</v>
       </c>
       <c r="C11">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -536,7 +536,7 @@
         <v>3</v>
       </c>
       <c r="C12">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -547,7 +547,7 @@
         <v>3</v>
       </c>
       <c r="C13">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -558,7 +558,7 @@
         <v>3</v>
       </c>
       <c r="C14">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -569,7 +569,7 @@
         <v>3</v>
       </c>
       <c r="C15">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -580,7 +580,7 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -591,7 +591,7 @@
         <v>3</v>
       </c>
       <c r="C17">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -602,7 +602,7 @@
         <v>3</v>
       </c>
       <c r="C18">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -613,7 +613,7 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -624,7 +624,7 @@
         <v>3</v>
       </c>
       <c r="C20">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -635,7 +635,7 @@
         <v>3</v>
       </c>
       <c r="C21">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -646,7 +646,7 @@
         <v>3</v>
       </c>
       <c r="C22">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -657,7 +657,7 @@
         <v>3</v>
       </c>
       <c r="C23">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -668,7 +668,7 @@
         <v>3</v>
       </c>
       <c r="C24">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -679,7 +679,7 @@
         <v>3</v>
       </c>
       <c r="C25">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -690,7 +690,7 @@
         <v>3</v>
       </c>
       <c r="C26">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -701,7 +701,7 @@
         <v>3</v>
       </c>
       <c r="C27">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -712,7 +712,7 @@
         <v>3</v>
       </c>
       <c r="C28">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -723,7 +723,7 @@
         <v>3</v>
       </c>
       <c r="C29">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -734,7 +734,7 @@
         <v>3</v>
       </c>
       <c r="C30">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -745,7 +745,7 @@
         <v>3</v>
       </c>
       <c r="C31">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -756,7 +756,7 @@
         <v>3</v>
       </c>
       <c r="C32">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -767,7 +767,7 @@
         <v>3</v>
       </c>
       <c r="C33">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -778,7 +778,7 @@
         <v>3</v>
       </c>
       <c r="C34">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -789,7 +789,7 @@
         <v>3</v>
       </c>
       <c r="C35">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -800,7 +800,7 @@
         <v>3</v>
       </c>
       <c r="C36">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -811,7 +811,7 @@
         <v>3</v>
       </c>
       <c r="C37">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -822,7 +822,7 @@
         <v>3</v>
       </c>
       <c r="C38">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -833,7 +833,7 @@
         <v>3</v>
       </c>
       <c r="C39">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -844,7 +844,7 @@
         <v>3</v>
       </c>
       <c r="C40">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -855,7 +855,7 @@
         <v>3</v>
       </c>
       <c r="C41">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -866,7 +866,7 @@
         <v>3</v>
       </c>
       <c r="C42">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -877,7 +877,7 @@
         <v>3</v>
       </c>
       <c r="C43">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -888,7 +888,7 @@
         <v>3</v>
       </c>
       <c r="C44">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -899,7 +899,7 @@
         <v>3</v>
       </c>
       <c r="C45">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -910,7 +910,7 @@
         <v>3</v>
       </c>
       <c r="C46">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -921,7 +921,7 @@
         <v>3</v>
       </c>
       <c r="C47">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -932,7 +932,7 @@
         <v>3</v>
       </c>
       <c r="C48">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -943,7 +943,7 @@
         <v>3</v>
       </c>
       <c r="C49">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -954,7 +954,7 @@
         <v>3</v>
       </c>
       <c r="C50">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -965,7 +965,7 @@
         <v>3</v>
       </c>
       <c r="C51">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -976,7 +976,7 @@
         <v>3</v>
       </c>
       <c r="C52">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -987,7 +987,7 @@
         <v>3</v>
       </c>
       <c r="C53">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -998,7 +998,7 @@
         <v>3</v>
       </c>
       <c r="C54">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1009,7 +1009,7 @@
         <v>3</v>
       </c>
       <c r="C55">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1020,7 +1020,7 @@
         <v>3</v>
       </c>
       <c r="C56">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1031,7 +1031,7 @@
         <v>3</v>
       </c>
       <c r="C57">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1042,7 +1042,7 @@
         <v>3</v>
       </c>
       <c r="C58">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -1053,7 +1053,7 @@
         <v>3</v>
       </c>
       <c r="C59">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -1064,7 +1064,7 @@
         <v>3</v>
       </c>
       <c r="C60">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -1075,7 +1075,7 @@
         <v>3</v>
       </c>
       <c r="C61">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -1086,7 +1086,7 @@
         <v>3</v>
       </c>
       <c r="C62">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -1097,7 +1097,7 @@
         <v>3</v>
       </c>
       <c r="C63">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -1108,7 +1108,7 @@
         <v>3</v>
       </c>
       <c r="C64">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -1119,7 +1119,7 @@
         <v>3</v>
       </c>
       <c r="C65">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -1130,7 +1130,7 @@
         <v>3</v>
       </c>
       <c r="C66">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -1141,7 +1141,7 @@
         <v>3</v>
       </c>
       <c r="C67">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -1152,7 +1152,7 @@
         <v>3</v>
       </c>
       <c r="C68">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -1163,7 +1163,7 @@
         <v>3</v>
       </c>
       <c r="C69">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -1174,7 +1174,7 @@
         <v>3</v>
       </c>
       <c r="C70">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -1185,7 +1185,7 @@
         <v>3</v>
       </c>
       <c r="C71">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -1196,7 +1196,7 @@
         <v>3</v>
       </c>
       <c r="C72">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -1207,7 +1207,7 @@
         <v>3</v>
       </c>
       <c r="C73">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -1218,7 +1218,7 @@
         <v>3</v>
       </c>
       <c r="C74">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -1229,7 +1229,7 @@
         <v>3</v>
       </c>
       <c r="C75">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -1240,7 +1240,7 @@
         <v>3</v>
       </c>
       <c r="C76">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -1251,7 +1251,7 @@
         <v>3</v>
       </c>
       <c r="C77">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -1262,7 +1262,7 @@
         <v>3</v>
       </c>
       <c r="C78">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -1273,7 +1273,7 @@
         <v>3</v>
       </c>
       <c r="C79">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -1284,7 +1284,7 @@
         <v>3</v>
       </c>
       <c r="C80">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -1295,7 +1295,7 @@
         <v>3</v>
       </c>
       <c r="C81">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -1306,7 +1306,7 @@
         <v>3</v>
       </c>
       <c r="C82">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -1317,7 +1317,7 @@
         <v>3</v>
       </c>
       <c r="C83">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -1328,7 +1328,7 @@
         <v>3</v>
       </c>
       <c r="C84">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -1339,7 +1339,7 @@
         <v>3</v>
       </c>
       <c r="C85">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -1350,7 +1350,7 @@
         <v>3</v>
       </c>
       <c r="C86">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -1361,7 +1361,7 @@
         <v>3</v>
       </c>
       <c r="C87">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -1372,7 +1372,7 @@
         <v>3</v>
       </c>
       <c r="C88">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -1383,7 +1383,7 @@
         <v>3</v>
       </c>
       <c r="C89">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -1394,7 +1394,7 @@
         <v>3</v>
       </c>
       <c r="C90">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -1405,7 +1405,7 @@
         <v>3</v>
       </c>
       <c r="C91">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -1416,7 +1416,7 @@
         <v>3</v>
       </c>
       <c r="C92">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -1427,7 +1427,7 @@
         <v>3</v>
       </c>
       <c r="C93">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -1438,7 +1438,7 @@
         <v>3</v>
       </c>
       <c r="C94">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -1449,7 +1449,7 @@
         <v>3</v>
       </c>
       <c r="C95">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -1460,7 +1460,7 @@
         <v>3</v>
       </c>
       <c r="C96">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -1471,7 +1471,7 @@
         <v>3</v>
       </c>
       <c r="C97">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -1482,7 +1482,7 @@
         <v>3</v>
       </c>
       <c r="C98">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -1493,7 +1493,7 @@
         <v>3</v>
       </c>
       <c r="C99">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -1504,7 +1504,7 @@
         <v>3</v>
       </c>
       <c r="C100">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -1515,7 +1515,7 @@
         <v>3</v>
       </c>
       <c r="C101">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -1526,7 +1526,7 @@
         <v>3</v>
       </c>
       <c r="C102">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -1537,7 +1537,7 @@
         <v>3</v>
       </c>
       <c r="C103">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -1548,7 +1548,7 @@
         <v>3</v>
       </c>
       <c r="C104">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -1559,7 +1559,7 @@
         <v>3</v>
       </c>
       <c r="C105">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -1570,7 +1570,7 @@
         <v>3</v>
       </c>
       <c r="C106">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -1581,7 +1581,7 @@
         <v>3</v>
       </c>
       <c r="C107">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -1592,7 +1592,7 @@
         <v>3</v>
       </c>
       <c r="C108">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -1603,7 +1603,7 @@
         <v>3</v>
       </c>
       <c r="C109">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -1614,7 +1614,7 @@
         <v>3</v>
       </c>
       <c r="C110">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -1625,7 +1625,7 @@
         <v>3</v>
       </c>
       <c r="C111">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -1636,7 +1636,7 @@
         <v>3</v>
       </c>
       <c r="C112">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -1647,7 +1647,7 @@
         <v>3</v>
       </c>
       <c r="C113">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -1658,7 +1658,7 @@
         <v>3</v>
       </c>
       <c r="C114">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -1669,7 +1669,7 @@
         <v>3</v>
       </c>
       <c r="C115">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -1680,7 +1680,7 @@
         <v>3</v>
       </c>
       <c r="C116">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -1691,7 +1691,7 @@
         <v>3</v>
       </c>
       <c r="C117">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -1702,7 +1702,7 @@
         <v>3</v>
       </c>
       <c r="C118">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -1713,7 +1713,7 @@
         <v>3</v>
       </c>
       <c r="C119">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -1724,7 +1724,7 @@
         <v>3</v>
       </c>
       <c r="C120">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -1735,7 +1735,7 @@
         <v>3</v>
       </c>
       <c r="C121">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -1746,7 +1746,7 @@
         <v>3</v>
       </c>
       <c r="C122">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
@@ -1757,7 +1757,7 @@
         <v>3</v>
       </c>
       <c r="C123">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
@@ -1768,7 +1768,7 @@
         <v>3</v>
       </c>
       <c r="C124">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
@@ -1779,7 +1779,7 @@
         <v>3</v>
       </c>
       <c r="C125">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
@@ -1790,7 +1790,7 @@
         <v>3</v>
       </c>
       <c r="C126">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
@@ -1801,7 +1801,7 @@
         <v>3</v>
       </c>
       <c r="C127">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
@@ -1812,7 +1812,7 @@
         <v>3</v>
       </c>
       <c r="C128">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
@@ -1823,7 +1823,7 @@
         <v>3</v>
       </c>
       <c r="C129">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
@@ -1834,7 +1834,7 @@
         <v>3</v>
       </c>
       <c r="C130">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
@@ -1845,7 +1845,7 @@
         <v>3</v>
       </c>
       <c r="C131">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
@@ -1856,7 +1856,7 @@
         <v>3</v>
       </c>
       <c r="C132">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
@@ -1867,7 +1867,7 @@
         <v>3</v>
       </c>
       <c r="C133">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
@@ -1878,7 +1878,7 @@
         <v>3</v>
       </c>
       <c r="C134">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
@@ -1889,7 +1889,7 @@
         <v>3</v>
       </c>
       <c r="C135">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
@@ -1900,7 +1900,7 @@
         <v>3</v>
       </c>
       <c r="C136">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
@@ -1911,7 +1911,7 @@
         <v>3</v>
       </c>
       <c r="C137">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
@@ -1922,7 +1922,7 @@
         <v>3</v>
       </c>
       <c r="C138">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
@@ -1933,7 +1933,7 @@
         <v>3</v>
       </c>
       <c r="C139">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
@@ -1944,7 +1944,7 @@
         <v>3</v>
       </c>
       <c r="C140">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
@@ -1955,7 +1955,7 @@
         <v>3</v>
       </c>
       <c r="C141">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
@@ -1966,7 +1966,7 @@
         <v>3</v>
       </c>
       <c r="C142">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
@@ -1977,7 +1977,7 @@
         <v>3</v>
       </c>
       <c r="C143">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
@@ -1988,7 +1988,7 @@
         <v>3</v>
       </c>
       <c r="C144">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
@@ -1999,7 +1999,7 @@
         <v>3</v>
       </c>
       <c r="C145">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
@@ -2010,7 +2010,7 @@
         <v>3</v>
       </c>
       <c r="C146">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
@@ -2021,7 +2021,7 @@
         <v>3</v>
       </c>
       <c r="C147">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
@@ -2032,7 +2032,7 @@
         <v>3</v>
       </c>
       <c r="C148">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
@@ -2043,7 +2043,7 @@
         <v>3</v>
       </c>
       <c r="C149">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
@@ -2054,7 +2054,7 @@
         <v>3</v>
       </c>
       <c r="C150">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
@@ -2065,7 +2065,7 @@
         <v>3</v>
       </c>
       <c r="C151">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
@@ -2076,7 +2076,7 @@
         <v>3</v>
       </c>
       <c r="C152">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
@@ -2087,7 +2087,7 @@
         <v>3</v>
       </c>
       <c r="C153">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
@@ -2098,7 +2098,7 @@
         <v>3</v>
       </c>
       <c r="C154">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
@@ -2109,7 +2109,7 @@
         <v>3</v>
       </c>
       <c r="C155">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
@@ -2120,7 +2120,7 @@
         <v>3</v>
       </c>
       <c r="C156">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
@@ -2131,7 +2131,7 @@
         <v>3</v>
       </c>
       <c r="C157">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
@@ -2142,7 +2142,7 @@
         <v>3</v>
       </c>
       <c r="C158">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
@@ -2153,7 +2153,7 @@
         <v>3</v>
       </c>
       <c r="C159">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
@@ -2164,7 +2164,7 @@
         <v>3</v>
       </c>
       <c r="C160">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
@@ -2175,7 +2175,7 @@
         <v>3</v>
       </c>
       <c r="C161">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
@@ -2186,7 +2186,7 @@
         <v>3</v>
       </c>
       <c r="C162">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
@@ -2197,7 +2197,7 @@
         <v>3</v>
       </c>
       <c r="C163">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
@@ -2208,7 +2208,7 @@
         <v>3</v>
       </c>
       <c r="C164">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
@@ -2219,7 +2219,7 @@
         <v>3</v>
       </c>
       <c r="C165">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
@@ -2230,7 +2230,7 @@
         <v>3</v>
       </c>
       <c r="C166">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
@@ -2241,7 +2241,7 @@
         <v>3</v>
       </c>
       <c r="C167">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
@@ -2252,7 +2252,7 @@
         <v>3</v>
       </c>
       <c r="C168">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
@@ -2263,7 +2263,7 @@
         <v>3</v>
       </c>
       <c r="C169">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
@@ -2274,7 +2274,7 @@
         <v>3</v>
       </c>
       <c r="C170">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
@@ -2285,7 +2285,7 @@
         <v>3</v>
       </c>
       <c r="C171">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
@@ -2296,7 +2296,7 @@
         <v>3</v>
       </c>
       <c r="C172">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
@@ -2307,7 +2307,7 @@
         <v>3</v>
       </c>
       <c r="C173">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
@@ -2318,7 +2318,7 @@
         <v>3</v>
       </c>
       <c r="C174">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
@@ -2329,7 +2329,7 @@
         <v>3</v>
       </c>
       <c r="C175">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
@@ -2340,7 +2340,7 @@
         <v>3</v>
       </c>
       <c r="C176">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
@@ -2351,7 +2351,7 @@
         <v>3</v>
       </c>
       <c r="C177">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
@@ -2362,7 +2362,7 @@
         <v>3</v>
       </c>
       <c r="C178">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
@@ -2373,7 +2373,7 @@
         <v>3</v>
       </c>
       <c r="C179">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
@@ -2384,7 +2384,7 @@
         <v>3</v>
       </c>
       <c r="C180">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
@@ -2395,7 +2395,7 @@
         <v>3</v>
       </c>
       <c r="C181">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
@@ -2406,7 +2406,7 @@
         <v>3</v>
       </c>
       <c r="C182">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
@@ -2417,7 +2417,7 @@
         <v>3</v>
       </c>
       <c r="C183">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
@@ -2428,7 +2428,7 @@
         <v>3</v>
       </c>
       <c r="C184">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
@@ -2439,7 +2439,7 @@
         <v>3</v>
       </c>
       <c r="C185">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
@@ -2450,7 +2450,7 @@
         <v>3</v>
       </c>
       <c r="C186">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
@@ -2461,7 +2461,7 @@
         <v>3</v>
       </c>
       <c r="C187">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
@@ -2472,7 +2472,7 @@
         <v>3</v>
       </c>
       <c r="C188">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
@@ -2483,7 +2483,7 @@
         <v>3</v>
       </c>
       <c r="C189">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
@@ -2494,7 +2494,7 @@
         <v>3</v>
       </c>
       <c r="C190">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
@@ -2505,7 +2505,7 @@
         <v>3</v>
       </c>
       <c r="C191">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
@@ -2516,7 +2516,7 @@
         <v>3</v>
       </c>
       <c r="C192">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
@@ -2527,7 +2527,7 @@
         <v>3</v>
       </c>
       <c r="C193">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
@@ -2538,7 +2538,7 @@
         <v>3</v>
       </c>
       <c r="C194">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
@@ -2549,7 +2549,7 @@
         <v>3</v>
       </c>
       <c r="C195">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
@@ -2560,7 +2560,7 @@
         <v>3</v>
       </c>
       <c r="C196">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
@@ -2571,7 +2571,7 @@
         <v>3</v>
       </c>
       <c r="C197">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
@@ -2582,7 +2582,7 @@
         <v>3</v>
       </c>
       <c r="C198">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
@@ -2593,7 +2593,7 @@
         <v>3</v>
       </c>
       <c r="C199">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
@@ -2604,7 +2604,7 @@
         <v>3</v>
       </c>
       <c r="C200">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
@@ -2615,7 +2615,7 @@
         <v>3</v>
       </c>
       <c r="C201">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
@@ -2626,7 +2626,7 @@
         <v>3</v>
       </c>
       <c r="C202">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
@@ -2637,7 +2637,7 @@
         <v>3</v>
       </c>
       <c r="C203">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
@@ -2648,7 +2648,7 @@
         <v>3</v>
       </c>
       <c r="C204">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
@@ -2659,7 +2659,7 @@
         <v>3</v>
       </c>
       <c r="C205">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
@@ -2670,7 +2670,7 @@
         <v>3</v>
       </c>
       <c r="C206">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
@@ -2681,7 +2681,7 @@
         <v>3</v>
       </c>
       <c r="C207">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
@@ -2692,7 +2692,7 @@
         <v>3</v>
       </c>
       <c r="C208">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
@@ -2703,7 +2703,7 @@
         <v>3</v>
       </c>
       <c r="C209">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
@@ -2714,7 +2714,7 @@
         <v>3</v>
       </c>
       <c r="C210">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
@@ -2725,7 +2725,7 @@
         <v>3</v>
       </c>
       <c r="C211">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
@@ -2736,7 +2736,7 @@
         <v>3</v>
       </c>
       <c r="C212">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
@@ -2747,7 +2747,7 @@
         <v>3</v>
       </c>
       <c r="C213">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
@@ -2758,7 +2758,7 @@
         <v>3</v>
       </c>
       <c r="C214">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
@@ -2769,7 +2769,7 @@
         <v>3</v>
       </c>
       <c r="C215">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
@@ -2780,7 +2780,7 @@
         <v>3</v>
       </c>
       <c r="C216">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
@@ -2791,7 +2791,7 @@
         <v>3</v>
       </c>
       <c r="C217">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
@@ -2802,7 +2802,7 @@
         <v>3</v>
       </c>
       <c r="C218">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
@@ -2813,7 +2813,7 @@
         <v>3</v>
       </c>
       <c r="C219">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
@@ -2824,7 +2824,7 @@
         <v>3</v>
       </c>
       <c r="C220">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
@@ -2835,7 +2835,7 @@
         <v>3</v>
       </c>
       <c r="C221">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
@@ -2846,7 +2846,7 @@
         <v>3</v>
       </c>
       <c r="C222">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
@@ -2857,7 +2857,7 @@
         <v>3</v>
       </c>
       <c r="C223">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
@@ -2868,7 +2868,7 @@
         <v>3</v>
       </c>
       <c r="C224">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
@@ -2879,7 +2879,7 @@
         <v>3</v>
       </c>
       <c r="C225">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
@@ -2890,7 +2890,7 @@
         <v>3</v>
       </c>
       <c r="C226">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
@@ -2901,7 +2901,7 @@
         <v>3</v>
       </c>
       <c r="C227">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
@@ -2912,7 +2912,7 @@
         <v>3</v>
       </c>
       <c r="C228">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
@@ -2923,7 +2923,7 @@
         <v>3</v>
       </c>
       <c r="C229">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
@@ -2934,7 +2934,7 @@
         <v>3</v>
       </c>
       <c r="C230">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
@@ -2945,7 +2945,7 @@
         <v>3</v>
       </c>
       <c r="C231">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
@@ -2956,7 +2956,7 @@
         <v>3</v>
       </c>
       <c r="C232">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
@@ -2967,7 +2967,7 @@
         <v>3</v>
       </c>
       <c r="C233">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
@@ -2978,7 +2978,7 @@
         <v>3</v>
       </c>
       <c r="C234">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
@@ -2989,7 +2989,7 @@
         <v>3</v>
       </c>
       <c r="C235">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
@@ -3000,7 +3000,7 @@
         <v>3</v>
       </c>
       <c r="C236">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
@@ -3011,7 +3011,7 @@
         <v>3</v>
       </c>
       <c r="C237">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
@@ -3022,7 +3022,7 @@
         <v>3</v>
       </c>
       <c r="C238">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
@@ -3033,7 +3033,7 @@
         <v>3</v>
       </c>
       <c r="C239">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
@@ -3044,7 +3044,7 @@
         <v>3</v>
       </c>
       <c r="C240">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
@@ -3055,7 +3055,7 @@
         <v>3</v>
       </c>
       <c r="C241">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
@@ -3066,7 +3066,7 @@
         <v>3</v>
       </c>
       <c r="C242">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
@@ -3077,7 +3077,7 @@
         <v>3</v>
       </c>
       <c r="C243">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
@@ -3088,7 +3088,7 @@
         <v>3</v>
       </c>
       <c r="C244">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
@@ -3099,7 +3099,7 @@
         <v>3</v>
       </c>
       <c r="C245">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
@@ -3110,7 +3110,7 @@
         <v>3</v>
       </c>
       <c r="C246">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
@@ -3121,7 +3121,7 @@
         <v>3</v>
       </c>
       <c r="C247">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
@@ -3132,7 +3132,7 @@
         <v>3</v>
       </c>
       <c r="C248">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
@@ -3143,7 +3143,7 @@
         <v>3</v>
       </c>
       <c r="C249">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
@@ -3154,7 +3154,7 @@
         <v>3</v>
       </c>
       <c r="C250">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
@@ -3165,7 +3165,7 @@
         <v>3</v>
       </c>
       <c r="C251">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
@@ -3176,7 +3176,7 @@
         <v>3</v>
       </c>
       <c r="C252">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
@@ -3187,7 +3187,7 @@
         <v>3</v>
       </c>
       <c r="C253">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
@@ -3198,7 +3198,7 @@
         <v>3</v>
       </c>
       <c r="C254">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
@@ -3209,7 +3209,7 @@
         <v>3</v>
       </c>
       <c r="C255">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
@@ -3220,7 +3220,7 @@
         <v>3</v>
       </c>
       <c r="C256">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
@@ -3231,7 +3231,7 @@
         <v>3</v>
       </c>
       <c r="C257">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
@@ -3242,7 +3242,7 @@
         <v>3</v>
       </c>
       <c r="C258">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
@@ -3253,7 +3253,7 @@
         <v>3</v>
       </c>
       <c r="C259">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
@@ -3264,7 +3264,7 @@
         <v>3</v>
       </c>
       <c r="C260">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
@@ -3275,7 +3275,7 @@
         <v>3</v>
       </c>
       <c r="C261">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
@@ -3286,7 +3286,7 @@
         <v>3</v>
       </c>
       <c r="C262">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
@@ -3297,7 +3297,7 @@
         <v>3</v>
       </c>
       <c r="C263">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
@@ -3308,7 +3308,7 @@
         <v>3</v>
       </c>
       <c r="C264">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
@@ -3319,7 +3319,7 @@
         <v>3</v>
       </c>
       <c r="C265">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
@@ -3330,7 +3330,7 @@
         <v>3</v>
       </c>
       <c r="C266">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
@@ -3341,7 +3341,7 @@
         <v>3</v>
       </c>
       <c r="C267">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
@@ -3352,7 +3352,7 @@
         <v>3</v>
       </c>
       <c r="C268">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
@@ -3363,7 +3363,7 @@
         <v>3</v>
       </c>
       <c r="C269">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
@@ -3374,7 +3374,7 @@
         <v>3</v>
       </c>
       <c r="C270">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
@@ -3385,7 +3385,7 @@
         <v>3</v>
       </c>
       <c r="C271">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
@@ -3396,7 +3396,7 @@
         <v>3</v>
       </c>
       <c r="C272">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
@@ -3407,7 +3407,7 @@
         <v>3</v>
       </c>
       <c r="C273">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
@@ -3418,7 +3418,7 @@
         <v>3</v>
       </c>
       <c r="C274">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
@@ -3429,7 +3429,7 @@
         <v>3</v>
       </c>
       <c r="C275">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
@@ -3440,7 +3440,7 @@
         <v>3</v>
       </c>
       <c r="C276">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
@@ -3451,7 +3451,7 @@
         <v>3</v>
       </c>
       <c r="C277">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
@@ -3462,7 +3462,7 @@
         <v>3</v>
       </c>
       <c r="C278">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
@@ -3473,7 +3473,7 @@
         <v>3</v>
       </c>
       <c r="C279">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
@@ -3484,7 +3484,7 @@
         <v>3</v>
       </c>
       <c r="C280">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
@@ -3495,7 +3495,7 @@
         <v>3</v>
       </c>
       <c r="C281">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
@@ -3506,7 +3506,7 @@
         <v>3</v>
       </c>
       <c r="C282">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
@@ -3517,7 +3517,7 @@
         <v>3</v>
       </c>
       <c r="C283">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
@@ -3528,7 +3528,7 @@
         <v>3</v>
       </c>
       <c r="C284">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
@@ -3539,7 +3539,7 @@
         <v>3</v>
       </c>
       <c r="C285">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
@@ -3550,7 +3550,7 @@
         <v>3</v>
       </c>
       <c r="C286">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.2">
@@ -3561,7 +3561,7 @@
         <v>3</v>
       </c>
       <c r="C287">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
@@ -3572,7 +3572,7 @@
         <v>3</v>
       </c>
       <c r="C288">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.2">
@@ -3583,7 +3583,7 @@
         <v>3</v>
       </c>
       <c r="C289">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.2">
@@ -3594,7 +3594,7 @@
         <v>3</v>
       </c>
       <c r="C290">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.2">
@@ -3605,7 +3605,7 @@
         <v>3</v>
       </c>
       <c r="C291">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.2">
@@ -3616,7 +3616,7 @@
         <v>3</v>
       </c>
       <c r="C292">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.2">
@@ -3627,7 +3627,7 @@
         <v>3</v>
       </c>
       <c r="C293">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.2">
@@ -3638,7 +3638,7 @@
         <v>3</v>
       </c>
       <c r="C294">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.2">
@@ -3649,7 +3649,7 @@
         <v>3</v>
       </c>
       <c r="C295">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.2">
@@ -3660,7 +3660,7 @@
         <v>3</v>
       </c>
       <c r="C296">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.2">
@@ -3671,7 +3671,7 @@
         <v>3</v>
       </c>
       <c r="C297">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.2">
@@ -3682,7 +3682,7 @@
         <v>3</v>
       </c>
       <c r="C298">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.2">
@@ -3693,7 +3693,7 @@
         <v>3</v>
       </c>
       <c r="C299">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.2">
@@ -3704,7 +3704,7 @@
         <v>3</v>
       </c>
       <c r="C300">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.2">
@@ -3715,7 +3715,7 @@
         <v>3</v>
       </c>
       <c r="C301">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.2">
@@ -3726,7 +3726,7 @@
         <v>3</v>
       </c>
       <c r="C302">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.2">
@@ -3737,7 +3737,7 @@
         <v>3</v>
       </c>
       <c r="C303">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.2">
@@ -3748,7 +3748,7 @@
         <v>3</v>
       </c>
       <c r="C304">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.2">
@@ -3759,7 +3759,7 @@
         <v>3</v>
       </c>
       <c r="C305">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.2">
@@ -3770,7 +3770,7 @@
         <v>3</v>
       </c>
       <c r="C306">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.2">
@@ -3781,7 +3781,7 @@
         <v>3</v>
       </c>
       <c r="C307">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.2">
@@ -3792,7 +3792,7 @@
         <v>3</v>
       </c>
       <c r="C308">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.2">
@@ -3803,7 +3803,7 @@
         <v>3</v>
       </c>
       <c r="C309">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.2">
@@ -3814,7 +3814,7 @@
         <v>3</v>
       </c>
       <c r="C310">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.2">
@@ -3825,7 +3825,7 @@
         <v>3</v>
       </c>
       <c r="C311">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.2">
@@ -3836,7 +3836,7 @@
         <v>3</v>
       </c>
       <c r="C312">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.2">
@@ -3847,7 +3847,7 @@
         <v>3</v>
       </c>
       <c r="C313">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.2">
@@ -3858,7 +3858,7 @@
         <v>3</v>
       </c>
       <c r="C314">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.2">
@@ -3869,7 +3869,7 @@
         <v>3</v>
       </c>
       <c r="C315">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.2">
@@ -3880,7 +3880,7 @@
         <v>3</v>
       </c>
       <c r="C316">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.2">
@@ -3891,7 +3891,7 @@
         <v>3</v>
       </c>
       <c r="C317">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.2">
@@ -3902,7 +3902,7 @@
         <v>3</v>
       </c>
       <c r="C318">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.2">
@@ -3913,7 +3913,7 @@
         <v>3</v>
       </c>
       <c r="C319">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.2">
@@ -3924,7 +3924,7 @@
         <v>3</v>
       </c>
       <c r="C320">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.2">
@@ -3935,7 +3935,7 @@
         <v>3</v>
       </c>
       <c r="C321">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.2">
@@ -3946,7 +3946,7 @@
         <v>3</v>
       </c>
       <c r="C322">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.2">
@@ -3957,7 +3957,7 @@
         <v>3</v>
       </c>
       <c r="C323">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.2">
@@ -3968,7 +3968,7 @@
         <v>3</v>
       </c>
       <c r="C324">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.2">
@@ -3979,7 +3979,7 @@
         <v>3</v>
       </c>
       <c r="C325">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.2">
@@ -3990,7 +3990,7 @@
         <v>3</v>
       </c>
       <c r="C326">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.2">
@@ -4001,7 +4001,7 @@
         <v>3</v>
       </c>
       <c r="C327">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.2">
@@ -4012,7 +4012,7 @@
         <v>3</v>
       </c>
       <c r="C328">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.2">
@@ -4023,7 +4023,7 @@
         <v>3</v>
       </c>
       <c r="C329">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.2">
@@ -4034,7 +4034,7 @@
         <v>3</v>
       </c>
       <c r="C330">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.2">
@@ -4045,7 +4045,7 @@
         <v>3</v>
       </c>
       <c r="C331">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.2">
@@ -4056,7 +4056,7 @@
         <v>3</v>
       </c>
       <c r="C332">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.2">
@@ -4067,7 +4067,7 @@
         <v>3</v>
       </c>
       <c r="C333">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.2">
@@ -4078,7 +4078,7 @@
         <v>3</v>
       </c>
       <c r="C334">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.2">
@@ -4089,7 +4089,7 @@
         <v>3</v>
       </c>
       <c r="C335">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.2">
@@ -4100,7 +4100,7 @@
         <v>3</v>
       </c>
       <c r="C336">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.2">
@@ -4111,7 +4111,7 @@
         <v>3</v>
       </c>
       <c r="C337">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.2">
@@ -4122,7 +4122,7 @@
         <v>3</v>
       </c>
       <c r="C338">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.2">
@@ -4133,7 +4133,7 @@
         <v>3</v>
       </c>
       <c r="C339">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.2">
@@ -4144,7 +4144,7 @@
         <v>3</v>
       </c>
       <c r="C340">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.2">
@@ -4155,7 +4155,7 @@
         <v>3</v>
       </c>
       <c r="C341">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.2">
@@ -4166,7 +4166,7 @@
         <v>3</v>
       </c>
       <c r="C342">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.2">
@@ -4177,7 +4177,7 @@
         <v>3</v>
       </c>
       <c r="C343">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.2">
@@ -4188,7 +4188,7 @@
         <v>3</v>
       </c>
       <c r="C344">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.2">
@@ -4199,7 +4199,7 @@
         <v>3</v>
       </c>
       <c r="C345">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.2">
@@ -4210,7 +4210,7 @@
         <v>3</v>
       </c>
       <c r="C346">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.2">
@@ -4221,7 +4221,7 @@
         <v>3</v>
       </c>
       <c r="C347">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.2">
@@ -4232,7 +4232,7 @@
         <v>3</v>
       </c>
       <c r="C348">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.2">
@@ -4243,7 +4243,7 @@
         <v>3</v>
       </c>
       <c r="C349">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.2">
@@ -4254,7 +4254,7 @@
         <v>3</v>
       </c>
       <c r="C350">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.2">
@@ -4265,7 +4265,7 @@
         <v>3</v>
       </c>
       <c r="C351">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.2">
@@ -4276,7 +4276,7 @@
         <v>3</v>
       </c>
       <c r="C352">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.2">
@@ -4287,7 +4287,7 @@
         <v>3</v>
       </c>
       <c r="C353">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.2">
@@ -4298,7 +4298,7 @@
         <v>3</v>
       </c>
       <c r="C354">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.2">
@@ -4309,7 +4309,7 @@
         <v>3</v>
       </c>
       <c r="C355">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.2">
@@ -4320,7 +4320,7 @@
         <v>3</v>
       </c>
       <c r="C356">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.2">
@@ -4331,7 +4331,7 @@
         <v>3</v>
       </c>
       <c r="C357">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.2">
@@ -4342,7 +4342,7 @@
         <v>3</v>
       </c>
       <c r="C358">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.2">
@@ -4353,7 +4353,7 @@
         <v>3</v>
       </c>
       <c r="C359">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.2">
@@ -4364,7 +4364,7 @@
         <v>3</v>
       </c>
       <c r="C360">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.2">
@@ -4375,7 +4375,7 @@
         <v>3</v>
       </c>
       <c r="C361">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.2">
@@ -4386,7 +4386,7 @@
         <v>3</v>
       </c>
       <c r="C362">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.2">
@@ -4397,7 +4397,7 @@
         <v>3</v>
       </c>
       <c r="C363">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.2">
@@ -4408,7 +4408,7 @@
         <v>3</v>
       </c>
       <c r="C364">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.2">
@@ -4419,7 +4419,7 @@
         <v>3</v>
       </c>
       <c r="C365">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.2">
@@ -4430,7 +4430,7 @@
         <v>3</v>
       </c>
       <c r="C366">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.2">
@@ -4441,7 +4441,7 @@
         <v>3</v>
       </c>
       <c r="C367">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.2">
@@ -4452,7 +4452,7 @@
         <v>3</v>
       </c>
       <c r="C368">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.2">
@@ -4463,7 +4463,7 @@
         <v>3</v>
       </c>
       <c r="C369">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.2">
@@ -4474,7 +4474,7 @@
         <v>3</v>
       </c>
       <c r="C370">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.2">
@@ -4485,7 +4485,7 @@
         <v>3</v>
       </c>
       <c r="C371">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.2">
@@ -4496,7 +4496,7 @@
         <v>3</v>
       </c>
       <c r="C372">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.2">
@@ -4507,7 +4507,7 @@
         <v>3</v>
       </c>
       <c r="C373">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.2">
@@ -4518,7 +4518,7 @@
         <v>3</v>
       </c>
       <c r="C374">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.2">
@@ -4529,7 +4529,7 @@
         <v>3</v>
       </c>
       <c r="C375">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.2">
@@ -4540,7 +4540,7 @@
         <v>3</v>
       </c>
       <c r="C376">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.2">
@@ -4551,7 +4551,7 @@
         <v>3</v>
       </c>
       <c r="C377">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.2">
@@ -4562,7 +4562,7 @@
         <v>3</v>
       </c>
       <c r="C378">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.2">
@@ -4573,7 +4573,7 @@
         <v>3</v>
       </c>
       <c r="C379">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.2">
@@ -4584,7 +4584,7 @@
         <v>3</v>
       </c>
       <c r="C380">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.2">
@@ -4595,7 +4595,7 @@
         <v>3</v>
       </c>
       <c r="C381">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.2">
@@ -4606,7 +4606,7 @@
         <v>3</v>
       </c>
       <c r="C382">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.2">
@@ -4617,7 +4617,7 @@
         <v>3</v>
       </c>
       <c r="C383">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.2">
@@ -4628,7 +4628,7 @@
         <v>3</v>
       </c>
       <c r="C384">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.2">
@@ -4639,7 +4639,7 @@
         <v>3</v>
       </c>
       <c r="C385">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.2">
@@ -4650,7 +4650,7 @@
         <v>3</v>
       </c>
       <c r="C386">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.2">
@@ -4661,7 +4661,7 @@
         <v>3</v>
       </c>
       <c r="C387">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.2">
@@ -4672,7 +4672,7 @@
         <v>3</v>
       </c>
       <c r="C388">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.2">
@@ -4683,7 +4683,7 @@
         <v>3</v>
       </c>
       <c r="C389">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.2">
@@ -4694,7 +4694,7 @@
         <v>3</v>
       </c>
       <c r="C390">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.2">
@@ -4705,7 +4705,7 @@
         <v>3</v>
       </c>
       <c r="C391">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.2">
@@ -4716,7 +4716,7 @@
         <v>3</v>
       </c>
       <c r="C392">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.2">
@@ -4727,7 +4727,7 @@
         <v>3</v>
       </c>
       <c r="C393">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.2">
@@ -4738,7 +4738,7 @@
         <v>3</v>
       </c>
       <c r="C394">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.2">
@@ -4749,7 +4749,7 @@
         <v>3</v>
       </c>
       <c r="C395">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.2">
@@ -4760,7 +4760,7 @@
         <v>3</v>
       </c>
       <c r="C396">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.2">
@@ -4771,7 +4771,7 @@
         <v>3</v>
       </c>
       <c r="C397">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.2">
@@ -4782,7 +4782,7 @@
         <v>3</v>
       </c>
       <c r="C398">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.2">
@@ -4793,7 +4793,7 @@
         <v>3</v>
       </c>
       <c r="C399">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.2">
@@ -4804,7 +4804,7 @@
         <v>3</v>
       </c>
       <c r="C400">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.2">
@@ -4815,7 +4815,7 @@
         <v>3</v>
       </c>
       <c r="C401">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.2">
@@ -4826,7 +4826,7 @@
         <v>3</v>
       </c>
       <c r="C402">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added parallel processing to post-processing of regional building stock tables
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Parameter_Building_Coverage.xlsx
+++ b/projects/test_building/input/Parameter_Building_Coverage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/test_building/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06751EFF-9A2E-5A40-803A-947879E591A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BC5491-F6C0-1141-8941-207E8B533C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A1:C402"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -426,7 +426,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -437,7 +437,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -448,7 +448,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -459,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -470,7 +470,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -481,7 +481,7 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -492,7 +492,7 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -503,7 +503,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -514,7 +514,7 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -525,7 +525,7 @@
         <v>3</v>
       </c>
       <c r="C11">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -536,7 +536,7 @@
         <v>3</v>
       </c>
       <c r="C12">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -547,7 +547,7 @@
         <v>3</v>
       </c>
       <c r="C13">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -558,7 +558,7 @@
         <v>3</v>
       </c>
       <c r="C14">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -569,7 +569,7 @@
         <v>3</v>
       </c>
       <c r="C15">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -580,7 +580,7 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -591,7 +591,7 @@
         <v>3</v>
       </c>
       <c r="C17">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -602,7 +602,7 @@
         <v>3</v>
       </c>
       <c r="C18">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -613,7 +613,7 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -624,7 +624,7 @@
         <v>3</v>
       </c>
       <c r="C20">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -635,7 +635,7 @@
         <v>3</v>
       </c>
       <c r="C21">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -646,7 +646,7 @@
         <v>3</v>
       </c>
       <c r="C22">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -657,7 +657,7 @@
         <v>3</v>
       </c>
       <c r="C23">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -668,7 +668,7 @@
         <v>3</v>
       </c>
       <c r="C24">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -679,7 +679,7 @@
         <v>3</v>
       </c>
       <c r="C25">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -690,7 +690,7 @@
         <v>3</v>
       </c>
       <c r="C26">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -701,7 +701,7 @@
         <v>3</v>
       </c>
       <c r="C27">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -712,7 +712,7 @@
         <v>3</v>
       </c>
       <c r="C28">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -723,7 +723,7 @@
         <v>3</v>
       </c>
       <c r="C29">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -734,7 +734,7 @@
         <v>3</v>
       </c>
       <c r="C30">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -745,7 +745,7 @@
         <v>3</v>
       </c>
       <c r="C31">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -756,7 +756,7 @@
         <v>3</v>
       </c>
       <c r="C32">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -767,7 +767,7 @@
         <v>3</v>
       </c>
       <c r="C33">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -778,7 +778,7 @@
         <v>3</v>
       </c>
       <c r="C34">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -789,7 +789,7 @@
         <v>3</v>
       </c>
       <c r="C35">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -800,7 +800,7 @@
         <v>3</v>
       </c>
       <c r="C36">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -811,7 +811,7 @@
         <v>3</v>
       </c>
       <c r="C37">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -822,7 +822,7 @@
         <v>3</v>
       </c>
       <c r="C38">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -833,7 +833,7 @@
         <v>3</v>
       </c>
       <c r="C39">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -844,7 +844,7 @@
         <v>3</v>
       </c>
       <c r="C40">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -855,7 +855,7 @@
         <v>3</v>
       </c>
       <c r="C41">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -866,7 +866,7 @@
         <v>3</v>
       </c>
       <c r="C42">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -877,7 +877,7 @@
         <v>3</v>
       </c>
       <c r="C43">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -888,7 +888,7 @@
         <v>3</v>
       </c>
       <c r="C44">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -899,7 +899,7 @@
         <v>3</v>
       </c>
       <c r="C45">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -910,7 +910,7 @@
         <v>3</v>
       </c>
       <c r="C46">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -921,7 +921,7 @@
         <v>3</v>
       </c>
       <c r="C47">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -932,7 +932,7 @@
         <v>3</v>
       </c>
       <c r="C48">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -943,7 +943,7 @@
         <v>3</v>
       </c>
       <c r="C49">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -954,7 +954,7 @@
         <v>3</v>
       </c>
       <c r="C50">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -965,7 +965,7 @@
         <v>3</v>
       </c>
       <c r="C51">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -976,7 +976,7 @@
         <v>3</v>
       </c>
       <c r="C52">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -987,7 +987,7 @@
         <v>3</v>
       </c>
       <c r="C53">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -998,7 +998,7 @@
         <v>3</v>
       </c>
       <c r="C54">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1009,7 +1009,7 @@
         <v>3</v>
       </c>
       <c r="C55">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1020,7 +1020,7 @@
         <v>3</v>
       </c>
       <c r="C56">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1031,7 +1031,7 @@
         <v>3</v>
       </c>
       <c r="C57">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1042,7 +1042,7 @@
         <v>3</v>
       </c>
       <c r="C58">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -1053,7 +1053,7 @@
         <v>3</v>
       </c>
       <c r="C59">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -1064,7 +1064,7 @@
         <v>3</v>
       </c>
       <c r="C60">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -1075,7 +1075,7 @@
         <v>3</v>
       </c>
       <c r="C61">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -1086,7 +1086,7 @@
         <v>3</v>
       </c>
       <c r="C62">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -1097,7 +1097,7 @@
         <v>3</v>
       </c>
       <c r="C63">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -1108,7 +1108,7 @@
         <v>3</v>
       </c>
       <c r="C64">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -1119,7 +1119,7 @@
         <v>3</v>
       </c>
       <c r="C65">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -1130,7 +1130,7 @@
         <v>3</v>
       </c>
       <c r="C66">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -1141,7 +1141,7 @@
         <v>3</v>
       </c>
       <c r="C67">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -1152,7 +1152,7 @@
         <v>3</v>
       </c>
       <c r="C68">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -1163,7 +1163,7 @@
         <v>3</v>
       </c>
       <c r="C69">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -1174,7 +1174,7 @@
         <v>3</v>
       </c>
       <c r="C70">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -1185,7 +1185,7 @@
         <v>3</v>
       </c>
       <c r="C71">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -1196,7 +1196,7 @@
         <v>3</v>
       </c>
       <c r="C72">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -1207,7 +1207,7 @@
         <v>3</v>
       </c>
       <c r="C73">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -1218,7 +1218,7 @@
         <v>3</v>
       </c>
       <c r="C74">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -1229,7 +1229,7 @@
         <v>3</v>
       </c>
       <c r="C75">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -1240,7 +1240,7 @@
         <v>3</v>
       </c>
       <c r="C76">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -1251,7 +1251,7 @@
         <v>3</v>
       </c>
       <c r="C77">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -1262,7 +1262,7 @@
         <v>3</v>
       </c>
       <c r="C78">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -1273,7 +1273,7 @@
         <v>3</v>
       </c>
       <c r="C79">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -1284,7 +1284,7 @@
         <v>3</v>
       </c>
       <c r="C80">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -1295,7 +1295,7 @@
         <v>3</v>
       </c>
       <c r="C81">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -1306,7 +1306,7 @@
         <v>3</v>
       </c>
       <c r="C82">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -1317,7 +1317,7 @@
         <v>3</v>
       </c>
       <c r="C83">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -1328,7 +1328,7 @@
         <v>3</v>
       </c>
       <c r="C84">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -1339,7 +1339,7 @@
         <v>3</v>
       </c>
       <c r="C85">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -1350,7 +1350,7 @@
         <v>3</v>
       </c>
       <c r="C86">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -1361,7 +1361,7 @@
         <v>3</v>
       </c>
       <c r="C87">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -1372,7 +1372,7 @@
         <v>3</v>
       </c>
       <c r="C88">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -1383,7 +1383,7 @@
         <v>3</v>
       </c>
       <c r="C89">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -1394,7 +1394,7 @@
         <v>3</v>
       </c>
       <c r="C90">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -1405,7 +1405,7 @@
         <v>3</v>
       </c>
       <c r="C91">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -1416,7 +1416,7 @@
         <v>3</v>
       </c>
       <c r="C92">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -1427,7 +1427,7 @@
         <v>3</v>
       </c>
       <c r="C93">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -1438,7 +1438,7 @@
         <v>3</v>
       </c>
       <c r="C94">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -1449,7 +1449,7 @@
         <v>3</v>
       </c>
       <c r="C95">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -1460,7 +1460,7 @@
         <v>3</v>
       </c>
       <c r="C96">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -1471,7 +1471,7 @@
         <v>3</v>
       </c>
       <c r="C97">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -1482,7 +1482,7 @@
         <v>3</v>
       </c>
       <c r="C98">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -1493,7 +1493,7 @@
         <v>3</v>
       </c>
       <c r="C99">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -1504,7 +1504,7 @@
         <v>3</v>
       </c>
       <c r="C100">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -1515,7 +1515,7 @@
         <v>3</v>
       </c>
       <c r="C101">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -1526,7 +1526,7 @@
         <v>3</v>
       </c>
       <c r="C102">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -1537,7 +1537,7 @@
         <v>3</v>
       </c>
       <c r="C103">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -1548,7 +1548,7 @@
         <v>3</v>
       </c>
       <c r="C104">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -1559,7 +1559,7 @@
         <v>3</v>
       </c>
       <c r="C105">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -1570,7 +1570,7 @@
         <v>3</v>
       </c>
       <c r="C106">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -1581,7 +1581,7 @@
         <v>3</v>
       </c>
       <c r="C107">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -1592,7 +1592,7 @@
         <v>3</v>
       </c>
       <c r="C108">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -1603,7 +1603,7 @@
         <v>3</v>
       </c>
       <c r="C109">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -1614,7 +1614,7 @@
         <v>3</v>
       </c>
       <c r="C110">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -1625,7 +1625,7 @@
         <v>3</v>
       </c>
       <c r="C111">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -1636,7 +1636,7 @@
         <v>3</v>
       </c>
       <c r="C112">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -1647,7 +1647,7 @@
         <v>3</v>
       </c>
       <c r="C113">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -1658,7 +1658,7 @@
         <v>3</v>
       </c>
       <c r="C114">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -1669,7 +1669,7 @@
         <v>3</v>
       </c>
       <c r="C115">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -1680,7 +1680,7 @@
         <v>3</v>
       </c>
       <c r="C116">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -1691,7 +1691,7 @@
         <v>3</v>
       </c>
       <c r="C117">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -1702,7 +1702,7 @@
         <v>3</v>
       </c>
       <c r="C118">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -1713,7 +1713,7 @@
         <v>3</v>
       </c>
       <c r="C119">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -1724,7 +1724,7 @@
         <v>3</v>
       </c>
       <c r="C120">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -1735,7 +1735,7 @@
         <v>3</v>
       </c>
       <c r="C121">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -1746,7 +1746,7 @@
         <v>3</v>
       </c>
       <c r="C122">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
@@ -1757,7 +1757,7 @@
         <v>3</v>
       </c>
       <c r="C123">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
@@ -1768,7 +1768,7 @@
         <v>3</v>
       </c>
       <c r="C124">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
@@ -1779,7 +1779,7 @@
         <v>3</v>
       </c>
       <c r="C125">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
@@ -1790,7 +1790,7 @@
         <v>3</v>
       </c>
       <c r="C126">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
@@ -1801,7 +1801,7 @@
         <v>3</v>
       </c>
       <c r="C127">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
@@ -1812,7 +1812,7 @@
         <v>3</v>
       </c>
       <c r="C128">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
@@ -1823,7 +1823,7 @@
         <v>3</v>
       </c>
       <c r="C129">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
@@ -1834,7 +1834,7 @@
         <v>3</v>
       </c>
       <c r="C130">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
@@ -1845,7 +1845,7 @@
         <v>3</v>
       </c>
       <c r="C131">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
@@ -1856,7 +1856,7 @@
         <v>3</v>
       </c>
       <c r="C132">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
@@ -1867,7 +1867,7 @@
         <v>3</v>
       </c>
       <c r="C133">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
@@ -1878,7 +1878,7 @@
         <v>3</v>
       </c>
       <c r="C134">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
@@ -1889,7 +1889,7 @@
         <v>3</v>
       </c>
       <c r="C135">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
@@ -1900,7 +1900,7 @@
         <v>3</v>
       </c>
       <c r="C136">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
@@ -1911,7 +1911,7 @@
         <v>3</v>
       </c>
       <c r="C137">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
@@ -1922,7 +1922,7 @@
         <v>3</v>
       </c>
       <c r="C138">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
@@ -1933,7 +1933,7 @@
         <v>3</v>
       </c>
       <c r="C139">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
@@ -1944,7 +1944,7 @@
         <v>3</v>
       </c>
       <c r="C140">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
@@ -1955,7 +1955,7 @@
         <v>3</v>
       </c>
       <c r="C141">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
@@ -1966,7 +1966,7 @@
         <v>3</v>
       </c>
       <c r="C142">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
@@ -1977,7 +1977,7 @@
         <v>3</v>
       </c>
       <c r="C143">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
@@ -1988,7 +1988,7 @@
         <v>3</v>
       </c>
       <c r="C144">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
@@ -1999,7 +1999,7 @@
         <v>3</v>
       </c>
       <c r="C145">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
@@ -2010,7 +2010,7 @@
         <v>3</v>
       </c>
       <c r="C146">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
@@ -2021,7 +2021,7 @@
         <v>3</v>
       </c>
       <c r="C147">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
@@ -2032,7 +2032,7 @@
         <v>3</v>
       </c>
       <c r="C148">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
@@ -2043,7 +2043,7 @@
         <v>3</v>
       </c>
       <c r="C149">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
@@ -2054,7 +2054,7 @@
         <v>3</v>
       </c>
       <c r="C150">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
@@ -2065,7 +2065,7 @@
         <v>3</v>
       </c>
       <c r="C151">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
@@ -2076,7 +2076,7 @@
         <v>3</v>
       </c>
       <c r="C152">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
@@ -2087,7 +2087,7 @@
         <v>3</v>
       </c>
       <c r="C153">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
@@ -2098,7 +2098,7 @@
         <v>3</v>
       </c>
       <c r="C154">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
@@ -2109,7 +2109,7 @@
         <v>3</v>
       </c>
       <c r="C155">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
@@ -2120,7 +2120,7 @@
         <v>3</v>
       </c>
       <c r="C156">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
@@ -2131,7 +2131,7 @@
         <v>3</v>
       </c>
       <c r="C157">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
@@ -2142,7 +2142,7 @@
         <v>3</v>
       </c>
       <c r="C158">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
@@ -2153,7 +2153,7 @@
         <v>3</v>
       </c>
       <c r="C159">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
@@ -2164,7 +2164,7 @@
         <v>3</v>
       </c>
       <c r="C160">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
@@ -2175,7 +2175,7 @@
         <v>3</v>
       </c>
       <c r="C161">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
@@ -2186,7 +2186,7 @@
         <v>3</v>
       </c>
       <c r="C162">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
@@ -2197,7 +2197,7 @@
         <v>3</v>
       </c>
       <c r="C163">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
@@ -2208,7 +2208,7 @@
         <v>3</v>
       </c>
       <c r="C164">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
@@ -2219,7 +2219,7 @@
         <v>3</v>
       </c>
       <c r="C165">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
@@ -2230,7 +2230,7 @@
         <v>3</v>
       </c>
       <c r="C166">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
@@ -2241,7 +2241,7 @@
         <v>3</v>
       </c>
       <c r="C167">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
@@ -2252,7 +2252,7 @@
         <v>3</v>
       </c>
       <c r="C168">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
@@ -2263,7 +2263,7 @@
         <v>3</v>
       </c>
       <c r="C169">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
@@ -2274,7 +2274,7 @@
         <v>3</v>
       </c>
       <c r="C170">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
@@ -2285,7 +2285,7 @@
         <v>3</v>
       </c>
       <c r="C171">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
@@ -2296,7 +2296,7 @@
         <v>3</v>
       </c>
       <c r="C172">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
@@ -2307,7 +2307,7 @@
         <v>3</v>
       </c>
       <c r="C173">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
@@ -2318,7 +2318,7 @@
         <v>3</v>
       </c>
       <c r="C174">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
@@ -2329,7 +2329,7 @@
         <v>3</v>
       </c>
       <c r="C175">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
@@ -2340,7 +2340,7 @@
         <v>3</v>
       </c>
       <c r="C176">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
@@ -2351,7 +2351,7 @@
         <v>3</v>
       </c>
       <c r="C177">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
@@ -2362,7 +2362,7 @@
         <v>3</v>
       </c>
       <c r="C178">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
@@ -2373,7 +2373,7 @@
         <v>3</v>
       </c>
       <c r="C179">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
@@ -2384,7 +2384,7 @@
         <v>3</v>
       </c>
       <c r="C180">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
@@ -2395,7 +2395,7 @@
         <v>3</v>
       </c>
       <c r="C181">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
@@ -2406,7 +2406,7 @@
         <v>3</v>
       </c>
       <c r="C182">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
@@ -2417,7 +2417,7 @@
         <v>3</v>
       </c>
       <c r="C183">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
@@ -2428,7 +2428,7 @@
         <v>3</v>
       </c>
       <c r="C184">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
@@ -2439,7 +2439,7 @@
         <v>3</v>
       </c>
       <c r="C185">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
@@ -2450,7 +2450,7 @@
         <v>3</v>
       </c>
       <c r="C186">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
@@ -2461,7 +2461,7 @@
         <v>3</v>
       </c>
       <c r="C187">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
@@ -2472,7 +2472,7 @@
         <v>3</v>
       </c>
       <c r="C188">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
@@ -2483,7 +2483,7 @@
         <v>3</v>
       </c>
       <c r="C189">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
@@ -2494,7 +2494,7 @@
         <v>3</v>
       </c>
       <c r="C190">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
@@ -2505,7 +2505,7 @@
         <v>3</v>
       </c>
       <c r="C191">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
@@ -2516,7 +2516,7 @@
         <v>3</v>
       </c>
       <c r="C192">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
@@ -2527,7 +2527,7 @@
         <v>3</v>
       </c>
       <c r="C193">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
@@ -2538,7 +2538,7 @@
         <v>3</v>
       </c>
       <c r="C194">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
@@ -2549,7 +2549,7 @@
         <v>3</v>
       </c>
       <c r="C195">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
@@ -2560,7 +2560,7 @@
         <v>3</v>
       </c>
       <c r="C196">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
@@ -2571,7 +2571,7 @@
         <v>3</v>
       </c>
       <c r="C197">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
@@ -2582,7 +2582,7 @@
         <v>3</v>
       </c>
       <c r="C198">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
@@ -2593,7 +2593,7 @@
         <v>3</v>
       </c>
       <c r="C199">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
@@ -2604,7 +2604,7 @@
         <v>3</v>
       </c>
       <c r="C200">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
@@ -2615,7 +2615,7 @@
         <v>3</v>
       </c>
       <c r="C201">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
@@ -2626,7 +2626,7 @@
         <v>3</v>
       </c>
       <c r="C202">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
@@ -2637,7 +2637,7 @@
         <v>3</v>
       </c>
       <c r="C203">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
@@ -2648,7 +2648,7 @@
         <v>3</v>
       </c>
       <c r="C204">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
@@ -2659,7 +2659,7 @@
         <v>3</v>
       </c>
       <c r="C205">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
@@ -2670,7 +2670,7 @@
         <v>3</v>
       </c>
       <c r="C206">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
@@ -2681,7 +2681,7 @@
         <v>3</v>
       </c>
       <c r="C207">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
@@ -2692,7 +2692,7 @@
         <v>3</v>
       </c>
       <c r="C208">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
@@ -2703,7 +2703,7 @@
         <v>3</v>
       </c>
       <c r="C209">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
@@ -2714,7 +2714,7 @@
         <v>3</v>
       </c>
       <c r="C210">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
@@ -2725,7 +2725,7 @@
         <v>3</v>
       </c>
       <c r="C211">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
@@ -2736,7 +2736,7 @@
         <v>3</v>
       </c>
       <c r="C212">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
@@ -2747,7 +2747,7 @@
         <v>3</v>
       </c>
       <c r="C213">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
@@ -2758,7 +2758,7 @@
         <v>3</v>
       </c>
       <c r="C214">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
@@ -2769,7 +2769,7 @@
         <v>3</v>
       </c>
       <c r="C215">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
@@ -2780,7 +2780,7 @@
         <v>3</v>
       </c>
       <c r="C216">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
@@ -2791,7 +2791,7 @@
         <v>3</v>
       </c>
       <c r="C217">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
@@ -2802,7 +2802,7 @@
         <v>3</v>
       </c>
       <c r="C218">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
@@ -2813,7 +2813,7 @@
         <v>3</v>
       </c>
       <c r="C219">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
@@ -2824,7 +2824,7 @@
         <v>3</v>
       </c>
       <c r="C220">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
@@ -2835,7 +2835,7 @@
         <v>3</v>
       </c>
       <c r="C221">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
@@ -2846,7 +2846,7 @@
         <v>3</v>
       </c>
       <c r="C222">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
@@ -2857,7 +2857,7 @@
         <v>3</v>
       </c>
       <c r="C223">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
@@ -2868,7 +2868,7 @@
         <v>3</v>
       </c>
       <c r="C224">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
@@ -2879,7 +2879,7 @@
         <v>3</v>
       </c>
       <c r="C225">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
@@ -2890,7 +2890,7 @@
         <v>3</v>
       </c>
       <c r="C226">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
@@ -2901,7 +2901,7 @@
         <v>3</v>
       </c>
       <c r="C227">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
@@ -2912,7 +2912,7 @@
         <v>3</v>
       </c>
       <c r="C228">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
@@ -2923,7 +2923,7 @@
         <v>3</v>
       </c>
       <c r="C229">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
@@ -2934,7 +2934,7 @@
         <v>3</v>
       </c>
       <c r="C230">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
@@ -2945,7 +2945,7 @@
         <v>3</v>
       </c>
       <c r="C231">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
@@ -2956,7 +2956,7 @@
         <v>3</v>
       </c>
       <c r="C232">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
@@ -2967,7 +2967,7 @@
         <v>3</v>
       </c>
       <c r="C233">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
@@ -2978,7 +2978,7 @@
         <v>3</v>
       </c>
       <c r="C234">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
@@ -2989,7 +2989,7 @@
         <v>3</v>
       </c>
       <c r="C235">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
@@ -3000,7 +3000,7 @@
         <v>3</v>
       </c>
       <c r="C236">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
@@ -3011,7 +3011,7 @@
         <v>3</v>
       </c>
       <c r="C237">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
@@ -3022,7 +3022,7 @@
         <v>3</v>
       </c>
       <c r="C238">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
@@ -3033,7 +3033,7 @@
         <v>3</v>
       </c>
       <c r="C239">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
@@ -3044,7 +3044,7 @@
         <v>3</v>
       </c>
       <c r="C240">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
@@ -3055,7 +3055,7 @@
         <v>3</v>
       </c>
       <c r="C241">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
@@ -3066,7 +3066,7 @@
         <v>3</v>
       </c>
       <c r="C242">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
@@ -3077,7 +3077,7 @@
         <v>3</v>
       </c>
       <c r="C243">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
@@ -3088,7 +3088,7 @@
         <v>3</v>
       </c>
       <c r="C244">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
@@ -3099,7 +3099,7 @@
         <v>3</v>
       </c>
       <c r="C245">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
@@ -3110,7 +3110,7 @@
         <v>3</v>
       </c>
       <c r="C246">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
@@ -3121,7 +3121,7 @@
         <v>3</v>
       </c>
       <c r="C247">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
@@ -3132,7 +3132,7 @@
         <v>3</v>
       </c>
       <c r="C248">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
@@ -3143,7 +3143,7 @@
         <v>3</v>
       </c>
       <c r="C249">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
@@ -3154,7 +3154,7 @@
         <v>3</v>
       </c>
       <c r="C250">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
@@ -3165,7 +3165,7 @@
         <v>3</v>
       </c>
       <c r="C251">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
@@ -3176,7 +3176,7 @@
         <v>3</v>
       </c>
       <c r="C252">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
@@ -3187,7 +3187,7 @@
         <v>3</v>
       </c>
       <c r="C253">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
@@ -3198,7 +3198,7 @@
         <v>3</v>
       </c>
       <c r="C254">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
@@ -3209,7 +3209,7 @@
         <v>3</v>
       </c>
       <c r="C255">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
@@ -3220,7 +3220,7 @@
         <v>3</v>
       </c>
       <c r="C256">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
@@ -3231,7 +3231,7 @@
         <v>3</v>
       </c>
       <c r="C257">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
@@ -3242,7 +3242,7 @@
         <v>3</v>
       </c>
       <c r="C258">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
@@ -3253,7 +3253,7 @@
         <v>3</v>
       </c>
       <c r="C259">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
@@ -3264,7 +3264,7 @@
         <v>3</v>
       </c>
       <c r="C260">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
@@ -3275,7 +3275,7 @@
         <v>3</v>
       </c>
       <c r="C261">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
@@ -3286,7 +3286,7 @@
         <v>3</v>
       </c>
       <c r="C262">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
@@ -3297,7 +3297,7 @@
         <v>3</v>
       </c>
       <c r="C263">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
@@ -3308,7 +3308,7 @@
         <v>3</v>
       </c>
       <c r="C264">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
@@ -3319,7 +3319,7 @@
         <v>3</v>
       </c>
       <c r="C265">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
@@ -3330,7 +3330,7 @@
         <v>3</v>
       </c>
       <c r="C266">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
@@ -3341,7 +3341,7 @@
         <v>3</v>
       </c>
       <c r="C267">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
@@ -3352,7 +3352,7 @@
         <v>3</v>
       </c>
       <c r="C268">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
@@ -3363,7 +3363,7 @@
         <v>3</v>
       </c>
       <c r="C269">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
@@ -3374,7 +3374,7 @@
         <v>3</v>
       </c>
       <c r="C270">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
@@ -3385,7 +3385,7 @@
         <v>3</v>
       </c>
       <c r="C271">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
@@ -3396,7 +3396,7 @@
         <v>3</v>
       </c>
       <c r="C272">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
@@ -3407,7 +3407,7 @@
         <v>3</v>
       </c>
       <c r="C273">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
@@ -3418,7 +3418,7 @@
         <v>3</v>
       </c>
       <c r="C274">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
@@ -3429,7 +3429,7 @@
         <v>3</v>
       </c>
       <c r="C275">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
@@ -3440,7 +3440,7 @@
         <v>3</v>
       </c>
       <c r="C276">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
@@ -3451,7 +3451,7 @@
         <v>3</v>
       </c>
       <c r="C277">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
@@ -3462,7 +3462,7 @@
         <v>3</v>
       </c>
       <c r="C278">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
@@ -3473,7 +3473,7 @@
         <v>3</v>
       </c>
       <c r="C279">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
@@ -3484,7 +3484,7 @@
         <v>3</v>
       </c>
       <c r="C280">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
@@ -3495,7 +3495,7 @@
         <v>3</v>
       </c>
       <c r="C281">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
@@ -3506,7 +3506,7 @@
         <v>3</v>
       </c>
       <c r="C282">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
@@ -3517,7 +3517,7 @@
         <v>3</v>
       </c>
       <c r="C283">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
@@ -3528,7 +3528,7 @@
         <v>3</v>
       </c>
       <c r="C284">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
@@ -3539,7 +3539,7 @@
         <v>3</v>
       </c>
       <c r="C285">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
@@ -3550,7 +3550,7 @@
         <v>3</v>
       </c>
       <c r="C286">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.2">
@@ -3561,7 +3561,7 @@
         <v>3</v>
       </c>
       <c r="C287">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
@@ -3572,7 +3572,7 @@
         <v>3</v>
       </c>
       <c r="C288">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.2">
@@ -3583,7 +3583,7 @@
         <v>3</v>
       </c>
       <c r="C289">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.2">
@@ -3594,7 +3594,7 @@
         <v>3</v>
       </c>
       <c r="C290">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.2">
@@ -3605,7 +3605,7 @@
         <v>3</v>
       </c>
       <c r="C291">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.2">
@@ -3616,7 +3616,7 @@
         <v>3</v>
       </c>
       <c r="C292">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.2">
@@ -3627,7 +3627,7 @@
         <v>3</v>
       </c>
       <c r="C293">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.2">
@@ -3638,7 +3638,7 @@
         <v>3</v>
       </c>
       <c r="C294">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.2">
@@ -3649,7 +3649,7 @@
         <v>3</v>
       </c>
       <c r="C295">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.2">
@@ -3660,7 +3660,7 @@
         <v>3</v>
       </c>
       <c r="C296">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.2">
@@ -3671,7 +3671,7 @@
         <v>3</v>
       </c>
       <c r="C297">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.2">
@@ -3682,7 +3682,7 @@
         <v>3</v>
       </c>
       <c r="C298">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.2">
@@ -3693,7 +3693,7 @@
         <v>3</v>
       </c>
       <c r="C299">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.2">
@@ -3704,7 +3704,7 @@
         <v>3</v>
       </c>
       <c r="C300">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.2">
@@ -3715,7 +3715,7 @@
         <v>3</v>
       </c>
       <c r="C301">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.2">
@@ -3726,7 +3726,7 @@
         <v>3</v>
       </c>
       <c r="C302">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.2">
@@ -3737,7 +3737,7 @@
         <v>3</v>
       </c>
       <c r="C303">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.2">
@@ -3748,7 +3748,7 @@
         <v>3</v>
       </c>
       <c r="C304">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.2">
@@ -3759,7 +3759,7 @@
         <v>3</v>
       </c>
       <c r="C305">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.2">
@@ -3770,7 +3770,7 @@
         <v>3</v>
       </c>
       <c r="C306">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.2">
@@ -3781,7 +3781,7 @@
         <v>3</v>
       </c>
       <c r="C307">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.2">
@@ -3792,7 +3792,7 @@
         <v>3</v>
       </c>
       <c r="C308">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.2">
@@ -3803,7 +3803,7 @@
         <v>3</v>
       </c>
       <c r="C309">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.2">
@@ -3814,7 +3814,7 @@
         <v>3</v>
       </c>
       <c r="C310">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.2">
@@ -3825,7 +3825,7 @@
         <v>3</v>
       </c>
       <c r="C311">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.2">
@@ -3836,7 +3836,7 @@
         <v>3</v>
       </c>
       <c r="C312">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.2">
@@ -3847,7 +3847,7 @@
         <v>3</v>
       </c>
       <c r="C313">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.2">
@@ -3858,7 +3858,7 @@
         <v>3</v>
       </c>
       <c r="C314">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.2">
@@ -3869,7 +3869,7 @@
         <v>3</v>
       </c>
       <c r="C315">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.2">
@@ -3880,7 +3880,7 @@
         <v>3</v>
       </c>
       <c r="C316">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.2">
@@ -3891,7 +3891,7 @@
         <v>3</v>
       </c>
       <c r="C317">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.2">
@@ -3902,7 +3902,7 @@
         <v>3</v>
       </c>
       <c r="C318">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.2">
@@ -3913,7 +3913,7 @@
         <v>3</v>
       </c>
       <c r="C319">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.2">
@@ -3924,7 +3924,7 @@
         <v>3</v>
       </c>
       <c r="C320">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.2">
@@ -3935,7 +3935,7 @@
         <v>3</v>
       </c>
       <c r="C321">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.2">
@@ -3946,7 +3946,7 @@
         <v>3</v>
       </c>
       <c r="C322">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.2">
@@ -3957,7 +3957,7 @@
         <v>3</v>
       </c>
       <c r="C323">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.2">
@@ -3968,7 +3968,7 @@
         <v>3</v>
       </c>
       <c r="C324">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.2">
@@ -3979,7 +3979,7 @@
         <v>3</v>
       </c>
       <c r="C325">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.2">
@@ -3990,7 +3990,7 @@
         <v>3</v>
       </c>
       <c r="C326">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.2">
@@ -4001,7 +4001,7 @@
         <v>3</v>
       </c>
       <c r="C327">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.2">
@@ -4012,7 +4012,7 @@
         <v>3</v>
       </c>
       <c r="C328">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.2">
@@ -4023,7 +4023,7 @@
         <v>3</v>
       </c>
       <c r="C329">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.2">
@@ -4034,7 +4034,7 @@
         <v>3</v>
       </c>
       <c r="C330">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.2">
@@ -4045,7 +4045,7 @@
         <v>3</v>
       </c>
       <c r="C331">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.2">
@@ -4056,7 +4056,7 @@
         <v>3</v>
       </c>
       <c r="C332">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.2">
@@ -4067,7 +4067,7 @@
         <v>3</v>
       </c>
       <c r="C333">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.2">
@@ -4078,7 +4078,7 @@
         <v>3</v>
       </c>
       <c r="C334">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.2">
@@ -4089,7 +4089,7 @@
         <v>3</v>
       </c>
       <c r="C335">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.2">
@@ -4100,7 +4100,7 @@
         <v>3</v>
       </c>
       <c r="C336">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.2">
@@ -4111,7 +4111,7 @@
         <v>3</v>
       </c>
       <c r="C337">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.2">
@@ -4122,7 +4122,7 @@
         <v>3</v>
       </c>
       <c r="C338">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.2">
@@ -4133,7 +4133,7 @@
         <v>3</v>
       </c>
       <c r="C339">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.2">
@@ -4144,7 +4144,7 @@
         <v>3</v>
       </c>
       <c r="C340">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.2">
@@ -4155,7 +4155,7 @@
         <v>3</v>
       </c>
       <c r="C341">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.2">
@@ -4166,7 +4166,7 @@
         <v>3</v>
       </c>
       <c r="C342">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.2">
@@ -4177,7 +4177,7 @@
         <v>3</v>
       </c>
       <c r="C343">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.2">
@@ -4188,7 +4188,7 @@
         <v>3</v>
       </c>
       <c r="C344">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.2">
@@ -4199,7 +4199,7 @@
         <v>3</v>
       </c>
       <c r="C345">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.2">
@@ -4210,7 +4210,7 @@
         <v>3</v>
       </c>
       <c r="C346">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.2">
@@ -4221,7 +4221,7 @@
         <v>3</v>
       </c>
       <c r="C347">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.2">
@@ -4232,7 +4232,7 @@
         <v>3</v>
       </c>
       <c r="C348">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.2">
@@ -4243,7 +4243,7 @@
         <v>3</v>
       </c>
       <c r="C349">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.2">
@@ -4254,7 +4254,7 @@
         <v>3</v>
       </c>
       <c r="C350">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.2">
@@ -4265,7 +4265,7 @@
         <v>3</v>
       </c>
       <c r="C351">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.2">
@@ -4276,7 +4276,7 @@
         <v>3</v>
       </c>
       <c r="C352">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.2">
@@ -4287,7 +4287,7 @@
         <v>3</v>
       </c>
       <c r="C353">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.2">
@@ -4298,7 +4298,7 @@
         <v>3</v>
       </c>
       <c r="C354">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.2">
@@ -4309,7 +4309,7 @@
         <v>3</v>
       </c>
       <c r="C355">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.2">
@@ -4320,7 +4320,7 @@
         <v>3</v>
       </c>
       <c r="C356">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.2">
@@ -4331,7 +4331,7 @@
         <v>3</v>
       </c>
       <c r="C357">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.2">
@@ -4342,7 +4342,7 @@
         <v>3</v>
       </c>
       <c r="C358">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.2">
@@ -4353,7 +4353,7 @@
         <v>3</v>
       </c>
       <c r="C359">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.2">
@@ -4364,7 +4364,7 @@
         <v>3</v>
       </c>
       <c r="C360">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.2">
@@ -4375,7 +4375,7 @@
         <v>3</v>
       </c>
       <c r="C361">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.2">
@@ -4386,7 +4386,7 @@
         <v>3</v>
       </c>
       <c r="C362">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.2">
@@ -4397,7 +4397,7 @@
         <v>3</v>
       </c>
       <c r="C363">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.2">
@@ -4408,7 +4408,7 @@
         <v>3</v>
       </c>
       <c r="C364">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.2">
@@ -4419,7 +4419,7 @@
         <v>3</v>
       </c>
       <c r="C365">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.2">
@@ -4430,7 +4430,7 @@
         <v>3</v>
       </c>
       <c r="C366">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.2">
@@ -4441,7 +4441,7 @@
         <v>3</v>
       </c>
       <c r="C367">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.2">
@@ -4452,7 +4452,7 @@
         <v>3</v>
       </c>
       <c r="C368">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.2">
@@ -4463,7 +4463,7 @@
         <v>3</v>
       </c>
       <c r="C369">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.2">
@@ -4474,7 +4474,7 @@
         <v>3</v>
       </c>
       <c r="C370">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.2">
@@ -4485,7 +4485,7 @@
         <v>3</v>
       </c>
       <c r="C371">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.2">
@@ -4496,7 +4496,7 @@
         <v>3</v>
       </c>
       <c r="C372">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.2">
@@ -4507,7 +4507,7 @@
         <v>3</v>
       </c>
       <c r="C373">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.2">
@@ -4518,7 +4518,7 @@
         <v>3</v>
       </c>
       <c r="C374">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.2">
@@ -4529,7 +4529,7 @@
         <v>3</v>
       </c>
       <c r="C375">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.2">
@@ -4540,7 +4540,7 @@
         <v>3</v>
       </c>
       <c r="C376">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.2">
@@ -4551,7 +4551,7 @@
         <v>3</v>
       </c>
       <c r="C377">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.2">
@@ -4562,7 +4562,7 @@
         <v>3</v>
       </c>
       <c r="C378">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.2">
@@ -4573,7 +4573,7 @@
         <v>3</v>
       </c>
       <c r="C379">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.2">
@@ -4584,7 +4584,7 @@
         <v>3</v>
       </c>
       <c r="C380">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.2">
@@ -4595,7 +4595,7 @@
         <v>3</v>
       </c>
       <c r="C381">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.2">
@@ -4606,7 +4606,7 @@
         <v>3</v>
       </c>
       <c r="C382">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.2">
@@ -4617,7 +4617,7 @@
         <v>3</v>
       </c>
       <c r="C383">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.2">
@@ -4628,7 +4628,7 @@
         <v>3</v>
       </c>
       <c r="C384">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.2">
@@ -4639,7 +4639,7 @@
         <v>3</v>
       </c>
       <c r="C385">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.2">
@@ -4650,7 +4650,7 @@
         <v>3</v>
       </c>
       <c r="C386">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.2">
@@ -4661,7 +4661,7 @@
         <v>3</v>
       </c>
       <c r="C387">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.2">
@@ -4672,7 +4672,7 @@
         <v>3</v>
       </c>
       <c r="C388">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.2">
@@ -4683,7 +4683,7 @@
         <v>3</v>
       </c>
       <c r="C389">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.2">
@@ -4694,7 +4694,7 @@
         <v>3</v>
       </c>
       <c r="C390">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.2">
@@ -4705,7 +4705,7 @@
         <v>3</v>
       </c>
       <c r="C391">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.2">
@@ -4716,7 +4716,7 @@
         <v>3</v>
       </c>
       <c r="C392">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.2">
@@ -4727,7 +4727,7 @@
         <v>3</v>
       </c>
       <c r="C393">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.2">
@@ -4738,7 +4738,7 @@
         <v>3</v>
       </c>
       <c r="C394">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.2">
@@ -4749,7 +4749,7 @@
         <v>3</v>
       </c>
       <c r="C395">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.2">
@@ -4760,7 +4760,7 @@
         <v>3</v>
       </c>
       <c r="C396">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.2">
@@ -4771,7 +4771,7 @@
         <v>3</v>
       </c>
       <c r="C397">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.2">
@@ -4782,7 +4782,7 @@
         <v>3</v>
       </c>
       <c r="C398">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.2">
@@ -4793,7 +4793,7 @@
         <v>3</v>
       </c>
       <c r="C399">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.2">
@@ -4804,7 +4804,7 @@
         <v>3</v>
       </c>
       <c r="C400">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.2">
@@ -4815,7 +4815,7 @@
         <v>3</v>
       </c>
       <c r="C401">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.2">
@@ -4826,7 +4826,7 @@
         <v>3</v>
       </c>
       <c r="C402">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made scenario tables id_scenario-dependent and defined scenario pathways for RokiG project. SimulatorScenarios now includes more id_scenario columns accordingly. also defined id_building_action=3 in relevant input tables for serial renovation.
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Parameter_Building_Coverage.xlsx
+++ b/projects/test_building/input/Parameter_Building_Coverage.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RenderNew\projects\test_building\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace_sia\RenderNew\projects\test_building\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -398,7 +398,7 @@
   <dimension ref="A1:C402"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C402"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,7 +425,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
test for heating system calibration
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Parameter_Building_Coverage.xlsx
+++ b/projects/test_building/input/Parameter_Building_Coverage.xlsx
@@ -398,7 +398,7 @@
   <dimension ref="A1:C402"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2:C402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,7 +436,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -447,7 +447,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -458,7 +458,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -469,7 +469,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -480,7 +480,7 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -491,7 +491,7 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -502,7 +502,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -513,7 +513,7 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -524,7 +524,7 @@
         <v>3</v>
       </c>
       <c r="C11">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -535,7 +535,7 @@
         <v>3</v>
       </c>
       <c r="C12">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -546,7 +546,7 @@
         <v>3</v>
       </c>
       <c r="C13">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -557,7 +557,7 @@
         <v>3</v>
       </c>
       <c r="C14">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -568,7 +568,7 @@
         <v>3</v>
       </c>
       <c r="C15">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -579,7 +579,7 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -590,7 +590,7 @@
         <v>3</v>
       </c>
       <c r="C17">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -601,7 +601,7 @@
         <v>3</v>
       </c>
       <c r="C18">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -623,7 +623,7 @@
         <v>3</v>
       </c>
       <c r="C20">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -634,7 +634,7 @@
         <v>3</v>
       </c>
       <c r="C21">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -645,7 +645,7 @@
         <v>3</v>
       </c>
       <c r="C22">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -656,7 +656,7 @@
         <v>3</v>
       </c>
       <c r="C23">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -667,7 +667,7 @@
         <v>3</v>
       </c>
       <c r="C24">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -678,7 +678,7 @@
         <v>3</v>
       </c>
       <c r="C25">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
         <v>3</v>
       </c>
       <c r="C26">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -700,7 +700,7 @@
         <v>3</v>
       </c>
       <c r="C27">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -711,7 +711,7 @@
         <v>3</v>
       </c>
       <c r="C28">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -722,7 +722,7 @@
         <v>3</v>
       </c>
       <c r="C29">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -733,7 +733,7 @@
         <v>3</v>
       </c>
       <c r="C30">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -744,7 +744,7 @@
         <v>3</v>
       </c>
       <c r="C31">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -755,7 +755,7 @@
         <v>3</v>
       </c>
       <c r="C32">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -766,7 +766,7 @@
         <v>3</v>
       </c>
       <c r="C33">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -777,7 +777,7 @@
         <v>3</v>
       </c>
       <c r="C34">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -788,7 +788,7 @@
         <v>3</v>
       </c>
       <c r="C35">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -799,7 +799,7 @@
         <v>3</v>
       </c>
       <c r="C36">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -810,7 +810,7 @@
         <v>3</v>
       </c>
       <c r="C37">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -821,7 +821,7 @@
         <v>3</v>
       </c>
       <c r="C38">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -832,7 +832,7 @@
         <v>3</v>
       </c>
       <c r="C39">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -843,7 +843,7 @@
         <v>3</v>
       </c>
       <c r="C40">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -854,7 +854,7 @@
         <v>3</v>
       </c>
       <c r="C41">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -865,7 +865,7 @@
         <v>3</v>
       </c>
       <c r="C42">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -876,7 +876,7 @@
         <v>3</v>
       </c>
       <c r="C43">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -887,7 +887,7 @@
         <v>3</v>
       </c>
       <c r="C44">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -898,7 +898,7 @@
         <v>3</v>
       </c>
       <c r="C45">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -909,7 +909,7 @@
         <v>3</v>
       </c>
       <c r="C46">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -920,7 +920,7 @@
         <v>3</v>
       </c>
       <c r="C47">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -931,7 +931,7 @@
         <v>3</v>
       </c>
       <c r="C48">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -942,7 +942,7 @@
         <v>3</v>
       </c>
       <c r="C49">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -953,7 +953,7 @@
         <v>3</v>
       </c>
       <c r="C50">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -964,7 +964,7 @@
         <v>3</v>
       </c>
       <c r="C51">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -975,7 +975,7 @@
         <v>3</v>
       </c>
       <c r="C52">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -986,7 +986,7 @@
         <v>3</v>
       </c>
       <c r="C53">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -997,7 +997,7 @@
         <v>3</v>
       </c>
       <c r="C54">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1008,7 +1008,7 @@
         <v>3</v>
       </c>
       <c r="C55">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1019,7 +1019,7 @@
         <v>3</v>
       </c>
       <c r="C56">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1030,7 +1030,7 @@
         <v>3</v>
       </c>
       <c r="C57">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1041,7 +1041,7 @@
         <v>3</v>
       </c>
       <c r="C58">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1052,7 +1052,7 @@
         <v>3</v>
       </c>
       <c r="C59">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1063,7 +1063,7 @@
         <v>3</v>
       </c>
       <c r="C60">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1074,7 +1074,7 @@
         <v>3</v>
       </c>
       <c r="C61">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1085,7 +1085,7 @@
         <v>3</v>
       </c>
       <c r="C62">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1096,7 +1096,7 @@
         <v>3</v>
       </c>
       <c r="C63">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1107,7 +1107,7 @@
         <v>3</v>
       </c>
       <c r="C64">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1118,7 +1118,7 @@
         <v>3</v>
       </c>
       <c r="C65">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1129,7 +1129,7 @@
         <v>3</v>
       </c>
       <c r="C66">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1140,7 +1140,7 @@
         <v>3</v>
       </c>
       <c r="C67">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1151,7 +1151,7 @@
         <v>3</v>
       </c>
       <c r="C68">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1162,7 +1162,7 @@
         <v>3</v>
       </c>
       <c r="C69">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1173,7 +1173,7 @@
         <v>3</v>
       </c>
       <c r="C70">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1184,7 +1184,7 @@
         <v>3</v>
       </c>
       <c r="C71">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1195,7 +1195,7 @@
         <v>3</v>
       </c>
       <c r="C72">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1206,7 +1206,7 @@
         <v>3</v>
       </c>
       <c r="C73">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1217,7 +1217,7 @@
         <v>3</v>
       </c>
       <c r="C74">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1228,7 +1228,7 @@
         <v>3</v>
       </c>
       <c r="C75">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1239,7 +1239,7 @@
         <v>3</v>
       </c>
       <c r="C76">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1250,7 +1250,7 @@
         <v>3</v>
       </c>
       <c r="C77">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1261,7 +1261,7 @@
         <v>3</v>
       </c>
       <c r="C78">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1272,7 +1272,7 @@
         <v>3</v>
       </c>
       <c r="C79">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1283,7 +1283,7 @@
         <v>3</v>
       </c>
       <c r="C80">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1294,7 +1294,7 @@
         <v>3</v>
       </c>
       <c r="C81">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -1305,7 +1305,7 @@
         <v>3</v>
       </c>
       <c r="C82">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1316,7 +1316,7 @@
         <v>3</v>
       </c>
       <c r="C83">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -1327,7 +1327,7 @@
         <v>3</v>
       </c>
       <c r="C84">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1338,7 +1338,7 @@
         <v>3</v>
       </c>
       <c r="C85">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1349,7 +1349,7 @@
         <v>3</v>
       </c>
       <c r="C86">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1360,7 +1360,7 @@
         <v>3</v>
       </c>
       <c r="C87">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -1371,7 +1371,7 @@
         <v>3</v>
       </c>
       <c r="C88">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -1382,7 +1382,7 @@
         <v>3</v>
       </c>
       <c r="C89">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -1393,7 +1393,7 @@
         <v>3</v>
       </c>
       <c r="C90">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -1404,7 +1404,7 @@
         <v>3</v>
       </c>
       <c r="C91">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -1415,7 +1415,7 @@
         <v>3</v>
       </c>
       <c r="C92">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -1426,7 +1426,7 @@
         <v>3</v>
       </c>
       <c r="C93">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -1437,7 +1437,7 @@
         <v>3</v>
       </c>
       <c r="C94">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -1448,7 +1448,7 @@
         <v>3</v>
       </c>
       <c r="C95">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -1459,7 +1459,7 @@
         <v>3</v>
       </c>
       <c r="C96">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -1470,7 +1470,7 @@
         <v>3</v>
       </c>
       <c r="C97">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -1481,7 +1481,7 @@
         <v>3</v>
       </c>
       <c r="C98">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -1492,7 +1492,7 @@
         <v>3</v>
       </c>
       <c r="C99">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -1503,7 +1503,7 @@
         <v>3</v>
       </c>
       <c r="C100">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -1514,7 +1514,7 @@
         <v>3</v>
       </c>
       <c r="C101">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -1525,7 +1525,7 @@
         <v>3</v>
       </c>
       <c r="C102">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -1536,7 +1536,7 @@
         <v>3</v>
       </c>
       <c r="C103">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -1547,7 +1547,7 @@
         <v>3</v>
       </c>
       <c r="C104">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -1558,7 +1558,7 @@
         <v>3</v>
       </c>
       <c r="C105">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -1569,7 +1569,7 @@
         <v>3</v>
       </c>
       <c r="C106">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -1580,7 +1580,7 @@
         <v>3</v>
       </c>
       <c r="C107">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -1591,7 +1591,7 @@
         <v>3</v>
       </c>
       <c r="C108">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -1602,7 +1602,7 @@
         <v>3</v>
       </c>
       <c r="C109">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -1613,7 +1613,7 @@
         <v>3</v>
       </c>
       <c r="C110">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -1624,7 +1624,7 @@
         <v>3</v>
       </c>
       <c r="C111">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -1635,7 +1635,7 @@
         <v>3</v>
       </c>
       <c r="C112">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -1646,7 +1646,7 @@
         <v>3</v>
       </c>
       <c r="C113">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -1657,7 +1657,7 @@
         <v>3</v>
       </c>
       <c r="C114">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -1668,7 +1668,7 @@
         <v>3</v>
       </c>
       <c r="C115">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -1679,7 +1679,7 @@
         <v>3</v>
       </c>
       <c r="C116">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -1690,7 +1690,7 @@
         <v>3</v>
       </c>
       <c r="C117">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -1701,7 +1701,7 @@
         <v>3</v>
       </c>
       <c r="C118">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -1712,7 +1712,7 @@
         <v>3</v>
       </c>
       <c r="C119">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -1723,7 +1723,7 @@
         <v>3</v>
       </c>
       <c r="C120">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -1734,7 +1734,7 @@
         <v>3</v>
       </c>
       <c r="C121">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -1745,7 +1745,7 @@
         <v>3</v>
       </c>
       <c r="C122">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -1756,7 +1756,7 @@
         <v>3</v>
       </c>
       <c r="C123">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -1767,7 +1767,7 @@
         <v>3</v>
       </c>
       <c r="C124">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -1778,7 +1778,7 @@
         <v>3</v>
       </c>
       <c r="C125">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -1789,7 +1789,7 @@
         <v>3</v>
       </c>
       <c r="C126">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -1800,7 +1800,7 @@
         <v>3</v>
       </c>
       <c r="C127">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -1811,7 +1811,7 @@
         <v>3</v>
       </c>
       <c r="C128">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -1822,7 +1822,7 @@
         <v>3</v>
       </c>
       <c r="C129">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -1833,7 +1833,7 @@
         <v>3</v>
       </c>
       <c r="C130">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -1844,7 +1844,7 @@
         <v>3</v>
       </c>
       <c r="C131">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -1855,7 +1855,7 @@
         <v>3</v>
       </c>
       <c r="C132">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -1866,7 +1866,7 @@
         <v>3</v>
       </c>
       <c r="C133">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -1877,7 +1877,7 @@
         <v>3</v>
       </c>
       <c r="C134">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -1888,7 +1888,7 @@
         <v>3</v>
       </c>
       <c r="C135">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -1899,7 +1899,7 @@
         <v>3</v>
       </c>
       <c r="C136">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -1910,7 +1910,7 @@
         <v>3</v>
       </c>
       <c r="C137">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -1921,7 +1921,7 @@
         <v>3</v>
       </c>
       <c r="C138">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -1932,7 +1932,7 @@
         <v>3</v>
       </c>
       <c r="C139">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -1943,7 +1943,7 @@
         <v>3</v>
       </c>
       <c r="C140">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -1954,7 +1954,7 @@
         <v>3</v>
       </c>
       <c r="C141">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -1965,7 +1965,7 @@
         <v>3</v>
       </c>
       <c r="C142">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -1976,7 +1976,7 @@
         <v>3</v>
       </c>
       <c r="C143">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -1987,7 +1987,7 @@
         <v>3</v>
       </c>
       <c r="C144">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -1998,7 +1998,7 @@
         <v>3</v>
       </c>
       <c r="C145">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -2009,7 +2009,7 @@
         <v>3</v>
       </c>
       <c r="C146">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -2020,7 +2020,7 @@
         <v>3</v>
       </c>
       <c r="C147">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -2031,7 +2031,7 @@
         <v>3</v>
       </c>
       <c r="C148">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -2042,7 +2042,7 @@
         <v>3</v>
       </c>
       <c r="C149">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -2053,7 +2053,7 @@
         <v>3</v>
       </c>
       <c r="C150">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -2064,7 +2064,7 @@
         <v>3</v>
       </c>
       <c r="C151">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -2075,7 +2075,7 @@
         <v>3</v>
       </c>
       <c r="C152">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -2086,7 +2086,7 @@
         <v>3</v>
       </c>
       <c r="C153">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -2097,7 +2097,7 @@
         <v>3</v>
       </c>
       <c r="C154">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -2108,7 +2108,7 @@
         <v>3</v>
       </c>
       <c r="C155">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -2119,7 +2119,7 @@
         <v>3</v>
       </c>
       <c r="C156">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -2130,7 +2130,7 @@
         <v>3</v>
       </c>
       <c r="C157">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -2141,7 +2141,7 @@
         <v>3</v>
       </c>
       <c r="C158">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -2152,7 +2152,7 @@
         <v>3</v>
       </c>
       <c r="C159">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -2163,7 +2163,7 @@
         <v>3</v>
       </c>
       <c r="C160">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -2174,7 +2174,7 @@
         <v>3</v>
       </c>
       <c r="C161">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -2185,7 +2185,7 @@
         <v>3</v>
       </c>
       <c r="C162">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -2196,7 +2196,7 @@
         <v>3</v>
       </c>
       <c r="C163">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -2207,7 +2207,7 @@
         <v>3</v>
       </c>
       <c r="C164">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -2218,7 +2218,7 @@
         <v>3</v>
       </c>
       <c r="C165">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -2229,7 +2229,7 @@
         <v>3</v>
       </c>
       <c r="C166">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -2240,7 +2240,7 @@
         <v>3</v>
       </c>
       <c r="C167">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -2251,7 +2251,7 @@
         <v>3</v>
       </c>
       <c r="C168">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -2262,7 +2262,7 @@
         <v>3</v>
       </c>
       <c r="C169">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -2273,7 +2273,7 @@
         <v>3</v>
       </c>
       <c r="C170">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -2284,7 +2284,7 @@
         <v>3</v>
       </c>
       <c r="C171">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -2295,7 +2295,7 @@
         <v>3</v>
       </c>
       <c r="C172">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -2306,7 +2306,7 @@
         <v>3</v>
       </c>
       <c r="C173">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -2317,7 +2317,7 @@
         <v>3</v>
       </c>
       <c r="C174">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -2328,7 +2328,7 @@
         <v>3</v>
       </c>
       <c r="C175">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -2339,7 +2339,7 @@
         <v>3</v>
       </c>
       <c r="C176">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -2350,7 +2350,7 @@
         <v>3</v>
       </c>
       <c r="C177">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -2361,7 +2361,7 @@
         <v>3</v>
       </c>
       <c r="C178">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -2372,7 +2372,7 @@
         <v>3</v>
       </c>
       <c r="C179">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -2383,7 +2383,7 @@
         <v>3</v>
       </c>
       <c r="C180">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -2394,7 +2394,7 @@
         <v>3</v>
       </c>
       <c r="C181">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -2405,7 +2405,7 @@
         <v>3</v>
       </c>
       <c r="C182">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -2416,7 +2416,7 @@
         <v>3</v>
       </c>
       <c r="C183">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -2427,7 +2427,7 @@
         <v>3</v>
       </c>
       <c r="C184">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -2438,7 +2438,7 @@
         <v>3</v>
       </c>
       <c r="C185">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -2449,7 +2449,7 @@
         <v>3</v>
       </c>
       <c r="C186">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -2460,7 +2460,7 @@
         <v>3</v>
       </c>
       <c r="C187">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -2471,7 +2471,7 @@
         <v>3</v>
       </c>
       <c r="C188">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -2482,7 +2482,7 @@
         <v>3</v>
       </c>
       <c r="C189">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -2493,7 +2493,7 @@
         <v>3</v>
       </c>
       <c r="C190">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -2504,7 +2504,7 @@
         <v>3</v>
       </c>
       <c r="C191">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -2515,7 +2515,7 @@
         <v>3</v>
       </c>
       <c r="C192">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -2526,7 +2526,7 @@
         <v>3</v>
       </c>
       <c r="C193">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -2537,7 +2537,7 @@
         <v>3</v>
       </c>
       <c r="C194">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -2548,7 +2548,7 @@
         <v>3</v>
       </c>
       <c r="C195">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -2559,7 +2559,7 @@
         <v>3</v>
       </c>
       <c r="C196">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -2570,7 +2570,7 @@
         <v>3</v>
       </c>
       <c r="C197">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -2581,7 +2581,7 @@
         <v>3</v>
       </c>
       <c r="C198">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -2592,7 +2592,7 @@
         <v>3</v>
       </c>
       <c r="C199">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -2603,7 +2603,7 @@
         <v>3</v>
       </c>
       <c r="C200">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -2614,7 +2614,7 @@
         <v>3</v>
       </c>
       <c r="C201">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -2625,7 +2625,7 @@
         <v>3</v>
       </c>
       <c r="C202">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -2636,7 +2636,7 @@
         <v>3</v>
       </c>
       <c r="C203">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -2647,7 +2647,7 @@
         <v>3</v>
       </c>
       <c r="C204">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -2658,7 +2658,7 @@
         <v>3</v>
       </c>
       <c r="C205">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -2669,7 +2669,7 @@
         <v>3</v>
       </c>
       <c r="C206">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -2680,7 +2680,7 @@
         <v>3</v>
       </c>
       <c r="C207">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -2691,7 +2691,7 @@
         <v>3</v>
       </c>
       <c r="C208">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -2702,7 +2702,7 @@
         <v>3</v>
       </c>
       <c r="C209">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -2713,7 +2713,7 @@
         <v>3</v>
       </c>
       <c r="C210">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -2724,7 +2724,7 @@
         <v>3</v>
       </c>
       <c r="C211">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -2735,7 +2735,7 @@
         <v>3</v>
       </c>
       <c r="C212">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -2746,7 +2746,7 @@
         <v>3</v>
       </c>
       <c r="C213">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -2757,7 +2757,7 @@
         <v>3</v>
       </c>
       <c r="C214">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -2768,7 +2768,7 @@
         <v>3</v>
       </c>
       <c r="C215">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
@@ -2779,7 +2779,7 @@
         <v>3</v>
       </c>
       <c r="C216">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
@@ -2790,7 +2790,7 @@
         <v>3</v>
       </c>
       <c r="C217">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -2801,7 +2801,7 @@
         <v>3</v>
       </c>
       <c r="C218">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -2812,7 +2812,7 @@
         <v>3</v>
       </c>
       <c r="C219">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -2823,7 +2823,7 @@
         <v>3</v>
       </c>
       <c r="C220">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -2834,7 +2834,7 @@
         <v>3</v>
       </c>
       <c r="C221">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -2845,7 +2845,7 @@
         <v>3</v>
       </c>
       <c r="C222">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -2856,7 +2856,7 @@
         <v>3</v>
       </c>
       <c r="C223">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -2867,7 +2867,7 @@
         <v>3</v>
       </c>
       <c r="C224">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -2878,7 +2878,7 @@
         <v>3</v>
       </c>
       <c r="C225">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -2889,7 +2889,7 @@
         <v>3</v>
       </c>
       <c r="C226">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
@@ -2900,7 +2900,7 @@
         <v>3</v>
       </c>
       <c r="C227">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -2911,7 +2911,7 @@
         <v>3</v>
       </c>
       <c r="C228">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -2922,7 +2922,7 @@
         <v>3</v>
       </c>
       <c r="C229">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -2933,7 +2933,7 @@
         <v>3</v>
       </c>
       <c r="C230">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -2944,7 +2944,7 @@
         <v>3</v>
       </c>
       <c r="C231">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -2955,7 +2955,7 @@
         <v>3</v>
       </c>
       <c r="C232">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -2966,7 +2966,7 @@
         <v>3</v>
       </c>
       <c r="C233">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -2977,7 +2977,7 @@
         <v>3</v>
       </c>
       <c r="C234">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -2988,7 +2988,7 @@
         <v>3</v>
       </c>
       <c r="C235">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -2999,7 +2999,7 @@
         <v>3</v>
       </c>
       <c r="C236">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -3010,7 +3010,7 @@
         <v>3</v>
       </c>
       <c r="C237">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -3021,7 +3021,7 @@
         <v>3</v>
       </c>
       <c r="C238">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -3032,7 +3032,7 @@
         <v>3</v>
       </c>
       <c r="C239">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -3043,7 +3043,7 @@
         <v>3</v>
       </c>
       <c r="C240">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -3054,7 +3054,7 @@
         <v>3</v>
       </c>
       <c r="C241">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
@@ -3065,7 +3065,7 @@
         <v>3</v>
       </c>
       <c r="C242">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -3076,7 +3076,7 @@
         <v>3</v>
       </c>
       <c r="C243">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -3087,7 +3087,7 @@
         <v>3</v>
       </c>
       <c r="C244">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -3098,7 +3098,7 @@
         <v>3</v>
       </c>
       <c r="C245">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -3109,7 +3109,7 @@
         <v>3</v>
       </c>
       <c r="C246">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
@@ -3120,7 +3120,7 @@
         <v>3</v>
       </c>
       <c r="C247">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
@@ -3131,7 +3131,7 @@
         <v>3</v>
       </c>
       <c r="C248">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
@@ -3142,7 +3142,7 @@
         <v>3</v>
       </c>
       <c r="C249">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
@@ -3153,7 +3153,7 @@
         <v>3</v>
       </c>
       <c r="C250">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
@@ -3164,7 +3164,7 @@
         <v>3</v>
       </c>
       <c r="C251">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -3175,7 +3175,7 @@
         <v>3</v>
       </c>
       <c r="C252">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
@@ -3186,7 +3186,7 @@
         <v>3</v>
       </c>
       <c r="C253">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
@@ -3197,7 +3197,7 @@
         <v>3</v>
       </c>
       <c r="C254">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
@@ -3208,7 +3208,7 @@
         <v>3</v>
       </c>
       <c r="C255">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
@@ -3219,7 +3219,7 @@
         <v>3</v>
       </c>
       <c r="C256">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
@@ -3230,7 +3230,7 @@
         <v>3</v>
       </c>
       <c r="C257">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -3241,7 +3241,7 @@
         <v>3</v>
       </c>
       <c r="C258">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
@@ -3252,7 +3252,7 @@
         <v>3</v>
       </c>
       <c r="C259">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
@@ -3263,7 +3263,7 @@
         <v>3</v>
       </c>
       <c r="C260">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -3274,7 +3274,7 @@
         <v>3</v>
       </c>
       <c r="C261">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -3285,7 +3285,7 @@
         <v>3</v>
       </c>
       <c r="C262">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -3296,7 +3296,7 @@
         <v>3</v>
       </c>
       <c r="C263">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
@@ -3307,7 +3307,7 @@
         <v>3</v>
       </c>
       <c r="C264">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -3318,7 +3318,7 @@
         <v>3</v>
       </c>
       <c r="C265">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -3329,7 +3329,7 @@
         <v>3</v>
       </c>
       <c r="C266">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
@@ -3340,7 +3340,7 @@
         <v>3</v>
       </c>
       <c r="C267">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -3351,7 +3351,7 @@
         <v>3</v>
       </c>
       <c r="C268">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -3362,7 +3362,7 @@
         <v>3</v>
       </c>
       <c r="C269">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
@@ -3373,7 +3373,7 @@
         <v>3</v>
       </c>
       <c r="C270">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -3384,7 +3384,7 @@
         <v>3</v>
       </c>
       <c r="C271">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -3395,7 +3395,7 @@
         <v>3</v>
       </c>
       <c r="C272">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -3406,7 +3406,7 @@
         <v>3</v>
       </c>
       <c r="C273">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -3417,7 +3417,7 @@
         <v>3</v>
       </c>
       <c r="C274">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -3428,7 +3428,7 @@
         <v>3</v>
       </c>
       <c r="C275">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -3439,7 +3439,7 @@
         <v>3</v>
       </c>
       <c r="C276">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -3450,7 +3450,7 @@
         <v>3</v>
       </c>
       <c r="C277">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -3461,7 +3461,7 @@
         <v>3</v>
       </c>
       <c r="C278">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -3472,7 +3472,7 @@
         <v>3</v>
       </c>
       <c r="C279">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -3483,7 +3483,7 @@
         <v>3</v>
       </c>
       <c r="C280">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -3494,7 +3494,7 @@
         <v>3</v>
       </c>
       <c r="C281">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -3505,7 +3505,7 @@
         <v>3</v>
       </c>
       <c r="C282">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
@@ -3516,7 +3516,7 @@
         <v>3</v>
       </c>
       <c r="C283">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -3527,7 +3527,7 @@
         <v>3</v>
       </c>
       <c r="C284">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -3538,7 +3538,7 @@
         <v>3</v>
       </c>
       <c r="C285">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -3549,7 +3549,7 @@
         <v>3</v>
       </c>
       <c r="C286">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -3560,7 +3560,7 @@
         <v>3</v>
       </c>
       <c r="C287">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -3571,7 +3571,7 @@
         <v>3</v>
       </c>
       <c r="C288">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
@@ -3582,7 +3582,7 @@
         <v>3</v>
       </c>
       <c r="C289">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
@@ -3593,7 +3593,7 @@
         <v>3</v>
       </c>
       <c r="C290">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
@@ -3604,7 +3604,7 @@
         <v>3</v>
       </c>
       <c r="C291">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
@@ -3615,7 +3615,7 @@
         <v>3</v>
       </c>
       <c r="C292">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
@@ -3626,7 +3626,7 @@
         <v>3</v>
       </c>
       <c r="C293">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
@@ -3637,7 +3637,7 @@
         <v>3</v>
       </c>
       <c r="C294">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
@@ -3648,7 +3648,7 @@
         <v>3</v>
       </c>
       <c r="C295">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
@@ -3659,7 +3659,7 @@
         <v>3</v>
       </c>
       <c r="C296">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
@@ -3670,7 +3670,7 @@
         <v>3</v>
       </c>
       <c r="C297">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
@@ -3681,7 +3681,7 @@
         <v>3</v>
       </c>
       <c r="C298">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
@@ -3692,7 +3692,7 @@
         <v>3</v>
       </c>
       <c r="C299">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
@@ -3703,7 +3703,7 @@
         <v>3</v>
       </c>
       <c r="C300">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
@@ -3714,7 +3714,7 @@
         <v>3</v>
       </c>
       <c r="C301">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
@@ -3725,7 +3725,7 @@
         <v>3</v>
       </c>
       <c r="C302">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
@@ -3736,7 +3736,7 @@
         <v>3</v>
       </c>
       <c r="C303">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
@@ -3747,7 +3747,7 @@
         <v>3</v>
       </c>
       <c r="C304">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
@@ -3758,7 +3758,7 @@
         <v>3</v>
       </c>
       <c r="C305">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
@@ -3769,7 +3769,7 @@
         <v>3</v>
       </c>
       <c r="C306">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
@@ -3780,7 +3780,7 @@
         <v>3</v>
       </c>
       <c r="C307">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
@@ -3791,7 +3791,7 @@
         <v>3</v>
       </c>
       <c r="C308">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
@@ -3802,7 +3802,7 @@
         <v>3</v>
       </c>
       <c r="C309">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
@@ -3813,7 +3813,7 @@
         <v>3</v>
       </c>
       <c r="C310">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
@@ -3824,7 +3824,7 @@
         <v>3</v>
       </c>
       <c r="C311">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
@@ -3835,7 +3835,7 @@
         <v>3</v>
       </c>
       <c r="C312">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
@@ -3846,7 +3846,7 @@
         <v>3</v>
       </c>
       <c r="C313">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
@@ -3857,7 +3857,7 @@
         <v>3</v>
       </c>
       <c r="C314">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
@@ -3868,7 +3868,7 @@
         <v>3</v>
       </c>
       <c r="C315">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
@@ -3879,7 +3879,7 @@
         <v>3</v>
       </c>
       <c r="C316">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
@@ -3890,7 +3890,7 @@
         <v>3</v>
       </c>
       <c r="C317">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
@@ -3901,7 +3901,7 @@
         <v>3</v>
       </c>
       <c r="C318">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
@@ -3912,7 +3912,7 @@
         <v>3</v>
       </c>
       <c r="C319">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
@@ -3923,7 +3923,7 @@
         <v>3</v>
       </c>
       <c r="C320">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
@@ -3934,7 +3934,7 @@
         <v>3</v>
       </c>
       <c r="C321">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
@@ -3945,7 +3945,7 @@
         <v>3</v>
       </c>
       <c r="C322">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
@@ -3956,7 +3956,7 @@
         <v>3</v>
       </c>
       <c r="C323">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
@@ -3967,7 +3967,7 @@
         <v>3</v>
       </c>
       <c r="C324">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
@@ -3978,7 +3978,7 @@
         <v>3</v>
       </c>
       <c r="C325">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
@@ -3989,7 +3989,7 @@
         <v>3</v>
       </c>
       <c r="C326">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
@@ -4000,7 +4000,7 @@
         <v>3</v>
       </c>
       <c r="C327">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
@@ -4011,7 +4011,7 @@
         <v>3</v>
       </c>
       <c r="C328">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
@@ -4022,7 +4022,7 @@
         <v>3</v>
       </c>
       <c r="C329">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
@@ -4033,7 +4033,7 @@
         <v>3</v>
       </c>
       <c r="C330">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
@@ -4044,7 +4044,7 @@
         <v>3</v>
       </c>
       <c r="C331">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
@@ -4055,7 +4055,7 @@
         <v>3</v>
       </c>
       <c r="C332">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
@@ -4066,7 +4066,7 @@
         <v>3</v>
       </c>
       <c r="C333">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
@@ -4077,7 +4077,7 @@
         <v>3</v>
       </c>
       <c r="C334">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
@@ -4088,7 +4088,7 @@
         <v>3</v>
       </c>
       <c r="C335">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
@@ -4099,7 +4099,7 @@
         <v>3</v>
       </c>
       <c r="C336">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
@@ -4110,7 +4110,7 @@
         <v>3</v>
       </c>
       <c r="C337">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
@@ -4121,7 +4121,7 @@
         <v>3</v>
       </c>
       <c r="C338">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
@@ -4132,7 +4132,7 @@
         <v>3</v>
       </c>
       <c r="C339">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
@@ -4143,7 +4143,7 @@
         <v>3</v>
       </c>
       <c r="C340">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
@@ -4154,7 +4154,7 @@
         <v>3</v>
       </c>
       <c r="C341">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
@@ -4165,7 +4165,7 @@
         <v>3</v>
       </c>
       <c r="C342">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
@@ -4176,7 +4176,7 @@
         <v>3</v>
       </c>
       <c r="C343">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.25">
@@ -4187,7 +4187,7 @@
         <v>3</v>
       </c>
       <c r="C344">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
@@ -4198,7 +4198,7 @@
         <v>3</v>
       </c>
       <c r="C345">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
@@ -4209,7 +4209,7 @@
         <v>3</v>
       </c>
       <c r="C346">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
@@ -4220,7 +4220,7 @@
         <v>3</v>
       </c>
       <c r="C347">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
@@ -4231,7 +4231,7 @@
         <v>3</v>
       </c>
       <c r="C348">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
@@ -4242,7 +4242,7 @@
         <v>3</v>
       </c>
       <c r="C349">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
@@ -4253,7 +4253,7 @@
         <v>3</v>
       </c>
       <c r="C350">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
@@ -4264,7 +4264,7 @@
         <v>3</v>
       </c>
       <c r="C351">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
@@ -4275,7 +4275,7 @@
         <v>3</v>
       </c>
       <c r="C352">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
@@ -4286,7 +4286,7 @@
         <v>3</v>
       </c>
       <c r="C353">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
@@ -4297,7 +4297,7 @@
         <v>3</v>
       </c>
       <c r="C354">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
@@ -4308,7 +4308,7 @@
         <v>3</v>
       </c>
       <c r="C355">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.25">
@@ -4319,7 +4319,7 @@
         <v>3</v>
       </c>
       <c r="C356">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
@@ -4330,7 +4330,7 @@
         <v>3</v>
       </c>
       <c r="C357">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.25">
@@ -4341,7 +4341,7 @@
         <v>3</v>
       </c>
       <c r="C358">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
@@ -4352,7 +4352,7 @@
         <v>3</v>
       </c>
       <c r="C359">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
@@ -4363,7 +4363,7 @@
         <v>3</v>
       </c>
       <c r="C360">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.25">
@@ -4374,7 +4374,7 @@
         <v>3</v>
       </c>
       <c r="C361">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.25">
@@ -4385,7 +4385,7 @@
         <v>3</v>
       </c>
       <c r="C362">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.25">
@@ -4396,7 +4396,7 @@
         <v>3</v>
       </c>
       <c r="C363">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
@@ -4407,7 +4407,7 @@
         <v>3</v>
       </c>
       <c r="C364">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
@@ -4418,7 +4418,7 @@
         <v>3</v>
       </c>
       <c r="C365">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
@@ -4429,7 +4429,7 @@
         <v>3</v>
       </c>
       <c r="C366">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
@@ -4440,7 +4440,7 @@
         <v>3</v>
       </c>
       <c r="C367">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.25">
@@ -4451,7 +4451,7 @@
         <v>3</v>
       </c>
       <c r="C368">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
@@ -4462,7 +4462,7 @@
         <v>3</v>
       </c>
       <c r="C369">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
@@ -4473,7 +4473,7 @@
         <v>3</v>
       </c>
       <c r="C370">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
@@ -4484,7 +4484,7 @@
         <v>3</v>
       </c>
       <c r="C371">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
@@ -4495,7 +4495,7 @@
         <v>3</v>
       </c>
       <c r="C372">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
@@ -4506,7 +4506,7 @@
         <v>3</v>
       </c>
       <c r="C373">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
@@ -4517,7 +4517,7 @@
         <v>3</v>
       </c>
       <c r="C374">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
@@ -4528,7 +4528,7 @@
         <v>3</v>
       </c>
       <c r="C375">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
@@ -4539,7 +4539,7 @@
         <v>3</v>
       </c>
       <c r="C376">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
@@ -4550,7 +4550,7 @@
         <v>3</v>
       </c>
       <c r="C377">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
@@ -4561,7 +4561,7 @@
         <v>3</v>
       </c>
       <c r="C378">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
@@ -4572,7 +4572,7 @@
         <v>3</v>
       </c>
       <c r="C379">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
@@ -4583,7 +4583,7 @@
         <v>3</v>
       </c>
       <c r="C380">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
@@ -4594,7 +4594,7 @@
         <v>3</v>
       </c>
       <c r="C381">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
@@ -4605,7 +4605,7 @@
         <v>3</v>
       </c>
       <c r="C382">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
@@ -4616,7 +4616,7 @@
         <v>3</v>
       </c>
       <c r="C383">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
@@ -4627,7 +4627,7 @@
         <v>3</v>
       </c>
       <c r="C384">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
@@ -4638,7 +4638,7 @@
         <v>3</v>
       </c>
       <c r="C385">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
@@ -4649,7 +4649,7 @@
         <v>3</v>
       </c>
       <c r="C386">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
@@ -4660,7 +4660,7 @@
         <v>3</v>
       </c>
       <c r="C387">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
@@ -4671,7 +4671,7 @@
         <v>3</v>
       </c>
       <c r="C388">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
@@ -4682,7 +4682,7 @@
         <v>3</v>
       </c>
       <c r="C389">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.25">
@@ -4693,7 +4693,7 @@
         <v>3</v>
       </c>
       <c r="C390">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
@@ -4704,7 +4704,7 @@
         <v>3</v>
       </c>
       <c r="C391">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">
@@ -4715,7 +4715,7 @@
         <v>3</v>
       </c>
       <c r="C392">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.25">
@@ -4726,7 +4726,7 @@
         <v>3</v>
       </c>
       <c r="C393">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.25">
@@ -4737,7 +4737,7 @@
         <v>3</v>
       </c>
       <c r="C394">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
@@ -4748,7 +4748,7 @@
         <v>3</v>
       </c>
       <c r="C395">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
@@ -4759,7 +4759,7 @@
         <v>3</v>
       </c>
       <c r="C396">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
@@ -4770,7 +4770,7 @@
         <v>3</v>
       </c>
       <c r="C397">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
@@ -4781,7 +4781,7 @@
         <v>3</v>
       </c>
       <c r="C398">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
@@ -4792,7 +4792,7 @@
         <v>3</v>
       </c>
       <c r="C399">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
@@ -4803,7 +4803,7 @@
         <v>3</v>
       </c>
       <c r="C400">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.25">
@@ -4814,7 +4814,7 @@
         <v>3</v>
       </c>
       <c r="C401">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.25">
@@ -4825,7 +4825,7 @@
         <v>3</v>
       </c>
       <c r="C402">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bring back input tables in development
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Parameter_Building_Coverage.xlsx
+++ b/projects/test_building/input/Parameter_Building_Coverage.xlsx
@@ -398,7 +398,7 @@
   <dimension ref="A1:C402"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C402"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -425,7 +425,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -436,7 +436,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -447,7 +447,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -458,7 +458,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -469,7 +469,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -480,7 +480,7 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -491,7 +491,7 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -502,7 +502,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -513,7 +513,7 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -524,7 +524,7 @@
         <v>3</v>
       </c>
       <c r="C11">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -535,7 +535,7 @@
         <v>3</v>
       </c>
       <c r="C12">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -546,7 +546,7 @@
         <v>3</v>
       </c>
       <c r="C13">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -557,7 +557,7 @@
         <v>3</v>
       </c>
       <c r="C14">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -568,7 +568,7 @@
         <v>3</v>
       </c>
       <c r="C15">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -579,7 +579,7 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -590,7 +590,7 @@
         <v>3</v>
       </c>
       <c r="C17">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -601,7 +601,7 @@
         <v>3</v>
       </c>
       <c r="C18">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -612,7 +612,7 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -623,7 +623,7 @@
         <v>3</v>
       </c>
       <c r="C20">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -634,7 +634,7 @@
         <v>3</v>
       </c>
       <c r="C21">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -645,7 +645,7 @@
         <v>3</v>
       </c>
       <c r="C22">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -656,7 +656,7 @@
         <v>3</v>
       </c>
       <c r="C23">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -667,7 +667,7 @@
         <v>3</v>
       </c>
       <c r="C24">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -678,7 +678,7 @@
         <v>3</v>
       </c>
       <c r="C25">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -689,7 +689,7 @@
         <v>3</v>
       </c>
       <c r="C26">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -700,7 +700,7 @@
         <v>3</v>
       </c>
       <c r="C27">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -711,7 +711,7 @@
         <v>3</v>
       </c>
       <c r="C28">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -722,7 +722,7 @@
         <v>3</v>
       </c>
       <c r="C29">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -733,7 +733,7 @@
         <v>3</v>
       </c>
       <c r="C30">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -744,7 +744,7 @@
         <v>3</v>
       </c>
       <c r="C31">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -755,7 +755,7 @@
         <v>3</v>
       </c>
       <c r="C32">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -766,7 +766,7 @@
         <v>3</v>
       </c>
       <c r="C33">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -777,7 +777,7 @@
         <v>3</v>
       </c>
       <c r="C34">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -788,7 +788,7 @@
         <v>3</v>
       </c>
       <c r="C35">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -799,7 +799,7 @@
         <v>3</v>
       </c>
       <c r="C36">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -810,7 +810,7 @@
         <v>3</v>
       </c>
       <c r="C37">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -821,7 +821,7 @@
         <v>3</v>
       </c>
       <c r="C38">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -832,7 +832,7 @@
         <v>3</v>
       </c>
       <c r="C39">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -843,7 +843,7 @@
         <v>3</v>
       </c>
       <c r="C40">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -854,7 +854,7 @@
         <v>3</v>
       </c>
       <c r="C41">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -865,7 +865,7 @@
         <v>3</v>
       </c>
       <c r="C42">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -876,7 +876,7 @@
         <v>3</v>
       </c>
       <c r="C43">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -887,7 +887,7 @@
         <v>3</v>
       </c>
       <c r="C44">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -898,7 +898,7 @@
         <v>3</v>
       </c>
       <c r="C45">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -909,7 +909,7 @@
         <v>3</v>
       </c>
       <c r="C46">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -920,7 +920,7 @@
         <v>3</v>
       </c>
       <c r="C47">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -931,7 +931,7 @@
         <v>3</v>
       </c>
       <c r="C48">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -942,7 +942,7 @@
         <v>3</v>
       </c>
       <c r="C49">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -953,7 +953,7 @@
         <v>3</v>
       </c>
       <c r="C50">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -964,7 +964,7 @@
         <v>3</v>
       </c>
       <c r="C51">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -975,7 +975,7 @@
         <v>3</v>
       </c>
       <c r="C52">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -986,7 +986,7 @@
         <v>3</v>
       </c>
       <c r="C53">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -997,7 +997,7 @@
         <v>3</v>
       </c>
       <c r="C54">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -1008,7 +1008,7 @@
         <v>3</v>
       </c>
       <c r="C55">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -1019,7 +1019,7 @@
         <v>3</v>
       </c>
       <c r="C56">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -1030,7 +1030,7 @@
         <v>3</v>
       </c>
       <c r="C57">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -1041,7 +1041,7 @@
         <v>3</v>
       </c>
       <c r="C58">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
@@ -1052,7 +1052,7 @@
         <v>3</v>
       </c>
       <c r="C59">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -1063,7 +1063,7 @@
         <v>3</v>
       </c>
       <c r="C60">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -1074,7 +1074,7 @@
         <v>3</v>
       </c>
       <c r="C61">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -1085,7 +1085,7 @@
         <v>3</v>
       </c>
       <c r="C62">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -1096,7 +1096,7 @@
         <v>3</v>
       </c>
       <c r="C63">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -1107,7 +1107,7 @@
         <v>3</v>
       </c>
       <c r="C64">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
@@ -1118,7 +1118,7 @@
         <v>3</v>
       </c>
       <c r="C65">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
@@ -1129,7 +1129,7 @@
         <v>3</v>
       </c>
       <c r="C66">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -1140,7 +1140,7 @@
         <v>3</v>
       </c>
       <c r="C67">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -1151,7 +1151,7 @@
         <v>3</v>
       </c>
       <c r="C68">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
@@ -1162,7 +1162,7 @@
         <v>3</v>
       </c>
       <c r="C69">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -1173,7 +1173,7 @@
         <v>3</v>
       </c>
       <c r="C70">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -1184,7 +1184,7 @@
         <v>3</v>
       </c>
       <c r="C71">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -1195,7 +1195,7 @@
         <v>3</v>
       </c>
       <c r="C72">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -1206,7 +1206,7 @@
         <v>3</v>
       </c>
       <c r="C73">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -1217,7 +1217,7 @@
         <v>3</v>
       </c>
       <c r="C74">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -1228,7 +1228,7 @@
         <v>3</v>
       </c>
       <c r="C75">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
@@ -1239,7 +1239,7 @@
         <v>3</v>
       </c>
       <c r="C76">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -1250,7 +1250,7 @@
         <v>3</v>
       </c>
       <c r="C77">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -1261,7 +1261,7 @@
         <v>3</v>
       </c>
       <c r="C78">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -1272,7 +1272,7 @@
         <v>3</v>
       </c>
       <c r="C79">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -1283,7 +1283,7 @@
         <v>3</v>
       </c>
       <c r="C80">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -1294,7 +1294,7 @@
         <v>3</v>
       </c>
       <c r="C81">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -1305,7 +1305,7 @@
         <v>3</v>
       </c>
       <c r="C82">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -1316,7 +1316,7 @@
         <v>3</v>
       </c>
       <c r="C83">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -1327,7 +1327,7 @@
         <v>3</v>
       </c>
       <c r="C84">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -1338,7 +1338,7 @@
         <v>3</v>
       </c>
       <c r="C85">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -1349,7 +1349,7 @@
         <v>3</v>
       </c>
       <c r="C86">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -1360,7 +1360,7 @@
         <v>3</v>
       </c>
       <c r="C87">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
@@ -1371,7 +1371,7 @@
         <v>3</v>
       </c>
       <c r="C88">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -1382,7 +1382,7 @@
         <v>3</v>
       </c>
       <c r="C89">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
@@ -1393,7 +1393,7 @@
         <v>3</v>
       </c>
       <c r="C90">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
@@ -1404,7 +1404,7 @@
         <v>3</v>
       </c>
       <c r="C91">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
@@ -1415,7 +1415,7 @@
         <v>3</v>
       </c>
       <c r="C92">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -1426,7 +1426,7 @@
         <v>3</v>
       </c>
       <c r="C93">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -1437,7 +1437,7 @@
         <v>3</v>
       </c>
       <c r="C94">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -1448,7 +1448,7 @@
         <v>3</v>
       </c>
       <c r="C95">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -1459,7 +1459,7 @@
         <v>3</v>
       </c>
       <c r="C96">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
@@ -1470,7 +1470,7 @@
         <v>3</v>
       </c>
       <c r="C97">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -1481,7 +1481,7 @@
         <v>3</v>
       </c>
       <c r="C98">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
@@ -1492,7 +1492,7 @@
         <v>3</v>
       </c>
       <c r="C99">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -1503,7 +1503,7 @@
         <v>3</v>
       </c>
       <c r="C100">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
@@ -1514,7 +1514,7 @@
         <v>3</v>
       </c>
       <c r="C101">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
@@ -1525,7 +1525,7 @@
         <v>3</v>
       </c>
       <c r="C102">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
@@ -1536,7 +1536,7 @@
         <v>3</v>
       </c>
       <c r="C103">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
@@ -1547,7 +1547,7 @@
         <v>3</v>
       </c>
       <c r="C104">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
@@ -1558,7 +1558,7 @@
         <v>3</v>
       </c>
       <c r="C105">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
@@ -1569,7 +1569,7 @@
         <v>3</v>
       </c>
       <c r="C106">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
@@ -1580,7 +1580,7 @@
         <v>3</v>
       </c>
       <c r="C107">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
@@ -1591,7 +1591,7 @@
         <v>3</v>
       </c>
       <c r="C108">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
@@ -1602,7 +1602,7 @@
         <v>3</v>
       </c>
       <c r="C109">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
@@ -1613,7 +1613,7 @@
         <v>3</v>
       </c>
       <c r="C110">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
@@ -1624,7 +1624,7 @@
         <v>3</v>
       </c>
       <c r="C111">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
@@ -1635,7 +1635,7 @@
         <v>3</v>
       </c>
       <c r="C112">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
@@ -1646,7 +1646,7 @@
         <v>3</v>
       </c>
       <c r="C113">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
@@ -1657,7 +1657,7 @@
         <v>3</v>
       </c>
       <c r="C114">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
@@ -1668,7 +1668,7 @@
         <v>3</v>
       </c>
       <c r="C115">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
@@ -1679,7 +1679,7 @@
         <v>3</v>
       </c>
       <c r="C116">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
@@ -1690,7 +1690,7 @@
         <v>3</v>
       </c>
       <c r="C117">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
@@ -1701,7 +1701,7 @@
         <v>3</v>
       </c>
       <c r="C118">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
@@ -1712,7 +1712,7 @@
         <v>3</v>
       </c>
       <c r="C119">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
@@ -1723,7 +1723,7 @@
         <v>3</v>
       </c>
       <c r="C120">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
@@ -1734,7 +1734,7 @@
         <v>3</v>
       </c>
       <c r="C121">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
@@ -1745,7 +1745,7 @@
         <v>3</v>
       </c>
       <c r="C122">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
@@ -1756,7 +1756,7 @@
         <v>3</v>
       </c>
       <c r="C123">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
@@ -1767,7 +1767,7 @@
         <v>3</v>
       </c>
       <c r="C124">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
@@ -1778,7 +1778,7 @@
         <v>3</v>
       </c>
       <c r="C125">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
@@ -1789,7 +1789,7 @@
         <v>3</v>
       </c>
       <c r="C126">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
@@ -1800,7 +1800,7 @@
         <v>3</v>
       </c>
       <c r="C127">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
@@ -1811,7 +1811,7 @@
         <v>3</v>
       </c>
       <c r="C128">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
@@ -1822,7 +1822,7 @@
         <v>3</v>
       </c>
       <c r="C129">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
@@ -1833,7 +1833,7 @@
         <v>3</v>
       </c>
       <c r="C130">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
@@ -1844,7 +1844,7 @@
         <v>3</v>
       </c>
       <c r="C131">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
@@ -1855,7 +1855,7 @@
         <v>3</v>
       </c>
       <c r="C132">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
@@ -1866,7 +1866,7 @@
         <v>3</v>
       </c>
       <c r="C133">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
@@ -1877,7 +1877,7 @@
         <v>3</v>
       </c>
       <c r="C134">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
@@ -1888,7 +1888,7 @@
         <v>3</v>
       </c>
       <c r="C135">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
@@ -1899,7 +1899,7 @@
         <v>3</v>
       </c>
       <c r="C136">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
@@ -1910,7 +1910,7 @@
         <v>3</v>
       </c>
       <c r="C137">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
@@ -1921,7 +1921,7 @@
         <v>3</v>
       </c>
       <c r="C138">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
@@ -1932,7 +1932,7 @@
         <v>3</v>
       </c>
       <c r="C139">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
@@ -1943,7 +1943,7 @@
         <v>3</v>
       </c>
       <c r="C140">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
@@ -1954,7 +1954,7 @@
         <v>3</v>
       </c>
       <c r="C141">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
@@ -1965,7 +1965,7 @@
         <v>3</v>
       </c>
       <c r="C142">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
@@ -1976,7 +1976,7 @@
         <v>3</v>
       </c>
       <c r="C143">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
@@ -1987,7 +1987,7 @@
         <v>3</v>
       </c>
       <c r="C144">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
@@ -1998,7 +1998,7 @@
         <v>3</v>
       </c>
       <c r="C145">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
@@ -2009,7 +2009,7 @@
         <v>3</v>
       </c>
       <c r="C146">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
@@ -2020,7 +2020,7 @@
         <v>3</v>
       </c>
       <c r="C147">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
@@ -2031,7 +2031,7 @@
         <v>3</v>
       </c>
       <c r="C148">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
@@ -2042,7 +2042,7 @@
         <v>3</v>
       </c>
       <c r="C149">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
@@ -2053,7 +2053,7 @@
         <v>3</v>
       </c>
       <c r="C150">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
@@ -2064,7 +2064,7 @@
         <v>3</v>
       </c>
       <c r="C151">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
@@ -2075,7 +2075,7 @@
         <v>3</v>
       </c>
       <c r="C152">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
@@ -2086,7 +2086,7 @@
         <v>3</v>
       </c>
       <c r="C153">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
@@ -2097,7 +2097,7 @@
         <v>3</v>
       </c>
       <c r="C154">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
@@ -2108,7 +2108,7 @@
         <v>3</v>
       </c>
       <c r="C155">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
@@ -2119,7 +2119,7 @@
         <v>3</v>
       </c>
       <c r="C156">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
@@ -2130,7 +2130,7 @@
         <v>3</v>
       </c>
       <c r="C157">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
@@ -2141,7 +2141,7 @@
         <v>3</v>
       </c>
       <c r="C158">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
@@ -2152,7 +2152,7 @@
         <v>3</v>
       </c>
       <c r="C159">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
@@ -2163,7 +2163,7 @@
         <v>3</v>
       </c>
       <c r="C160">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
@@ -2174,7 +2174,7 @@
         <v>3</v>
       </c>
       <c r="C161">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
@@ -2185,7 +2185,7 @@
         <v>3</v>
       </c>
       <c r="C162">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
@@ -2196,7 +2196,7 @@
         <v>3</v>
       </c>
       <c r="C163">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
@@ -2207,7 +2207,7 @@
         <v>3</v>
       </c>
       <c r="C164">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
@@ -2218,7 +2218,7 @@
         <v>3</v>
       </c>
       <c r="C165">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
@@ -2229,7 +2229,7 @@
         <v>3</v>
       </c>
       <c r="C166">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
@@ -2240,7 +2240,7 @@
         <v>3</v>
       </c>
       <c r="C167">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
@@ -2251,7 +2251,7 @@
         <v>3</v>
       </c>
       <c r="C168">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
@@ -2262,7 +2262,7 @@
         <v>3</v>
       </c>
       <c r="C169">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
@@ -2273,7 +2273,7 @@
         <v>3</v>
       </c>
       <c r="C170">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
@@ -2284,7 +2284,7 @@
         <v>3</v>
       </c>
       <c r="C171">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
@@ -2295,7 +2295,7 @@
         <v>3</v>
       </c>
       <c r="C172">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
@@ -2306,7 +2306,7 @@
         <v>3</v>
       </c>
       <c r="C173">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
@@ -2317,7 +2317,7 @@
         <v>3</v>
       </c>
       <c r="C174">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
@@ -2328,7 +2328,7 @@
         <v>3</v>
       </c>
       <c r="C175">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
@@ -2339,7 +2339,7 @@
         <v>3</v>
       </c>
       <c r="C176">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
@@ -2350,7 +2350,7 @@
         <v>3</v>
       </c>
       <c r="C177">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
@@ -2361,7 +2361,7 @@
         <v>3</v>
       </c>
       <c r="C178">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
@@ -2372,7 +2372,7 @@
         <v>3</v>
       </c>
       <c r="C179">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
@@ -2383,7 +2383,7 @@
         <v>3</v>
       </c>
       <c r="C180">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
@@ -2394,7 +2394,7 @@
         <v>3</v>
       </c>
       <c r="C181">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
@@ -2405,7 +2405,7 @@
         <v>3</v>
       </c>
       <c r="C182">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
@@ -2416,7 +2416,7 @@
         <v>3</v>
       </c>
       <c r="C183">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
@@ -2427,7 +2427,7 @@
         <v>3</v>
       </c>
       <c r="C184">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
@@ -2438,7 +2438,7 @@
         <v>3</v>
       </c>
       <c r="C185">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
@@ -2449,7 +2449,7 @@
         <v>3</v>
       </c>
       <c r="C186">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
@@ -2460,7 +2460,7 @@
         <v>3</v>
       </c>
       <c r="C187">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
@@ -2471,7 +2471,7 @@
         <v>3</v>
       </c>
       <c r="C188">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">
@@ -2482,7 +2482,7 @@
         <v>3</v>
       </c>
       <c r="C189">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.35">
@@ -2493,7 +2493,7 @@
         <v>3</v>
       </c>
       <c r="C190">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.35">
@@ -2504,7 +2504,7 @@
         <v>3</v>
       </c>
       <c r="C191">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.35">
@@ -2515,7 +2515,7 @@
         <v>3</v>
       </c>
       <c r="C192">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.35">
@@ -2526,7 +2526,7 @@
         <v>3</v>
       </c>
       <c r="C193">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.35">
@@ -2537,7 +2537,7 @@
         <v>3</v>
       </c>
       <c r="C194">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.35">
@@ -2548,7 +2548,7 @@
         <v>3</v>
       </c>
       <c r="C195">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.35">
@@ -2559,7 +2559,7 @@
         <v>3</v>
       </c>
       <c r="C196">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.35">
@@ -2570,7 +2570,7 @@
         <v>3</v>
       </c>
       <c r="C197">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.35">
@@ -2581,7 +2581,7 @@
         <v>3</v>
       </c>
       <c r="C198">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.35">
@@ -2592,7 +2592,7 @@
         <v>3</v>
       </c>
       <c r="C199">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.35">
@@ -2603,7 +2603,7 @@
         <v>3</v>
       </c>
       <c r="C200">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.35">
@@ -2614,7 +2614,7 @@
         <v>3</v>
       </c>
       <c r="C201">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.35">
@@ -2625,7 +2625,7 @@
         <v>3</v>
       </c>
       <c r="C202">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.35">
@@ -2636,7 +2636,7 @@
         <v>3</v>
       </c>
       <c r="C203">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.35">
@@ -2647,7 +2647,7 @@
         <v>3</v>
       </c>
       <c r="C204">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.35">
@@ -2658,7 +2658,7 @@
         <v>3</v>
       </c>
       <c r="C205">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.35">
@@ -2669,7 +2669,7 @@
         <v>3</v>
       </c>
       <c r="C206">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.35">
@@ -2680,7 +2680,7 @@
         <v>3</v>
       </c>
       <c r="C207">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.35">
@@ -2691,7 +2691,7 @@
         <v>3</v>
       </c>
       <c r="C208">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.35">
@@ -2702,7 +2702,7 @@
         <v>3</v>
       </c>
       <c r="C209">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.35">
@@ -2713,7 +2713,7 @@
         <v>3</v>
       </c>
       <c r="C210">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.35">
@@ -2724,7 +2724,7 @@
         <v>3</v>
       </c>
       <c r="C211">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.35">
@@ -2735,7 +2735,7 @@
         <v>3</v>
       </c>
       <c r="C212">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.35">
@@ -2746,7 +2746,7 @@
         <v>3</v>
       </c>
       <c r="C213">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.35">
@@ -2757,7 +2757,7 @@
         <v>3</v>
       </c>
       <c r="C214">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.35">
@@ -2768,7 +2768,7 @@
         <v>3</v>
       </c>
       <c r="C215">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.35">
@@ -2779,7 +2779,7 @@
         <v>3</v>
       </c>
       <c r="C216">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.35">
@@ -2790,7 +2790,7 @@
         <v>3</v>
       </c>
       <c r="C217">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.35">
@@ -2801,7 +2801,7 @@
         <v>3</v>
       </c>
       <c r="C218">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.35">
@@ -2812,7 +2812,7 @@
         <v>3</v>
       </c>
       <c r="C219">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.35">
@@ -2823,7 +2823,7 @@
         <v>3</v>
       </c>
       <c r="C220">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.35">
@@ -2834,7 +2834,7 @@
         <v>3</v>
       </c>
       <c r="C221">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.35">
@@ -2845,7 +2845,7 @@
         <v>3</v>
       </c>
       <c r="C222">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.35">
@@ -2856,7 +2856,7 @@
         <v>3</v>
       </c>
       <c r="C223">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.35">
@@ -2867,7 +2867,7 @@
         <v>3</v>
       </c>
       <c r="C224">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.35">
@@ -2878,7 +2878,7 @@
         <v>3</v>
       </c>
       <c r="C225">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.35">
@@ -2889,7 +2889,7 @@
         <v>3</v>
       </c>
       <c r="C226">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.35">
@@ -2900,7 +2900,7 @@
         <v>3</v>
       </c>
       <c r="C227">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.35">
@@ -2911,7 +2911,7 @@
         <v>3</v>
       </c>
       <c r="C228">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.35">
@@ -2922,7 +2922,7 @@
         <v>3</v>
       </c>
       <c r="C229">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.35">
@@ -2933,7 +2933,7 @@
         <v>3</v>
       </c>
       <c r="C230">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.35">
@@ -2944,7 +2944,7 @@
         <v>3</v>
       </c>
       <c r="C231">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.35">
@@ -2955,7 +2955,7 @@
         <v>3</v>
       </c>
       <c r="C232">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.35">
@@ -2966,7 +2966,7 @@
         <v>3</v>
       </c>
       <c r="C233">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.35">
@@ -2977,7 +2977,7 @@
         <v>3</v>
       </c>
       <c r="C234">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.35">
@@ -2988,7 +2988,7 @@
         <v>3</v>
       </c>
       <c r="C235">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.35">
@@ -2999,7 +2999,7 @@
         <v>3</v>
       </c>
       <c r="C236">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.35">
@@ -3010,7 +3010,7 @@
         <v>3</v>
       </c>
       <c r="C237">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.35">
@@ -3021,7 +3021,7 @@
         <v>3</v>
       </c>
       <c r="C238">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.35">
@@ -3032,7 +3032,7 @@
         <v>3</v>
       </c>
       <c r="C239">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.35">
@@ -3043,7 +3043,7 @@
         <v>3</v>
       </c>
       <c r="C240">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.35">
@@ -3054,7 +3054,7 @@
         <v>3</v>
       </c>
       <c r="C241">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.35">
@@ -3065,7 +3065,7 @@
         <v>3</v>
       </c>
       <c r="C242">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.35">
@@ -3076,7 +3076,7 @@
         <v>3</v>
       </c>
       <c r="C243">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.35">
@@ -3087,7 +3087,7 @@
         <v>3</v>
       </c>
       <c r="C244">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.35">
@@ -3098,7 +3098,7 @@
         <v>3</v>
       </c>
       <c r="C245">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.35">
@@ -3109,7 +3109,7 @@
         <v>3</v>
       </c>
       <c r="C246">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.35">
@@ -3120,7 +3120,7 @@
         <v>3</v>
       </c>
       <c r="C247">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.35">
@@ -3131,7 +3131,7 @@
         <v>3</v>
       </c>
       <c r="C248">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.35">
@@ -3142,7 +3142,7 @@
         <v>3</v>
       </c>
       <c r="C249">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.35">
@@ -3153,7 +3153,7 @@
         <v>3</v>
       </c>
       <c r="C250">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.35">
@@ -3164,7 +3164,7 @@
         <v>3</v>
       </c>
       <c r="C251">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.35">
@@ -3175,7 +3175,7 @@
         <v>3</v>
       </c>
       <c r="C252">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.35">
@@ -3186,7 +3186,7 @@
         <v>3</v>
       </c>
       <c r="C253">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.35">
@@ -3197,7 +3197,7 @@
         <v>3</v>
       </c>
       <c r="C254">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.35">
@@ -3208,7 +3208,7 @@
         <v>3</v>
       </c>
       <c r="C255">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.35">
@@ -3219,7 +3219,7 @@
         <v>3</v>
       </c>
       <c r="C256">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.35">
@@ -3230,7 +3230,7 @@
         <v>3</v>
       </c>
       <c r="C257">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.35">
@@ -3241,7 +3241,7 @@
         <v>3</v>
       </c>
       <c r="C258">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.35">
@@ -3252,7 +3252,7 @@
         <v>3</v>
       </c>
       <c r="C259">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.35">
@@ -3263,7 +3263,7 @@
         <v>3</v>
       </c>
       <c r="C260">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.35">
@@ -3274,7 +3274,7 @@
         <v>3</v>
       </c>
       <c r="C261">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.35">
@@ -3285,7 +3285,7 @@
         <v>3</v>
       </c>
       <c r="C262">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.35">
@@ -3296,7 +3296,7 @@
         <v>3</v>
       </c>
       <c r="C263">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.35">
@@ -3307,7 +3307,7 @@
         <v>3</v>
       </c>
       <c r="C264">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.35">
@@ -3318,7 +3318,7 @@
         <v>3</v>
       </c>
       <c r="C265">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.35">
@@ -3329,7 +3329,7 @@
         <v>3</v>
       </c>
       <c r="C266">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.35">
@@ -3340,7 +3340,7 @@
         <v>3</v>
       </c>
       <c r="C267">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.35">
@@ -3351,7 +3351,7 @@
         <v>3</v>
       </c>
       <c r="C268">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.35">
@@ -3362,7 +3362,7 @@
         <v>3</v>
       </c>
       <c r="C269">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.35">
@@ -3373,7 +3373,7 @@
         <v>3</v>
       </c>
       <c r="C270">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.35">
@@ -3384,7 +3384,7 @@
         <v>3</v>
       </c>
       <c r="C271">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.35">
@@ -3395,7 +3395,7 @@
         <v>3</v>
       </c>
       <c r="C272">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.35">
@@ -3406,7 +3406,7 @@
         <v>3</v>
       </c>
       <c r="C273">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.35">
@@ -3417,7 +3417,7 @@
         <v>3</v>
       </c>
       <c r="C274">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.35">
@@ -3428,7 +3428,7 @@
         <v>3</v>
       </c>
       <c r="C275">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.35">
@@ -3439,7 +3439,7 @@
         <v>3</v>
       </c>
       <c r="C276">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.35">
@@ -3450,7 +3450,7 @@
         <v>3</v>
       </c>
       <c r="C277">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.35">
@@ -3461,7 +3461,7 @@
         <v>3</v>
       </c>
       <c r="C278">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.35">
@@ -3472,7 +3472,7 @@
         <v>3</v>
       </c>
       <c r="C279">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.35">
@@ -3483,7 +3483,7 @@
         <v>3</v>
       </c>
       <c r="C280">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.35">
@@ -3494,7 +3494,7 @@
         <v>3</v>
       </c>
       <c r="C281">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.35">
@@ -3505,7 +3505,7 @@
         <v>3</v>
       </c>
       <c r="C282">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.35">
@@ -3516,7 +3516,7 @@
         <v>3</v>
       </c>
       <c r="C283">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.35">
@@ -3527,7 +3527,7 @@
         <v>3</v>
       </c>
       <c r="C284">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.35">
@@ -3538,7 +3538,7 @@
         <v>3</v>
       </c>
       <c r="C285">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.35">
@@ -3549,7 +3549,7 @@
         <v>3</v>
       </c>
       <c r="C286">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.35">
@@ -3560,7 +3560,7 @@
         <v>3</v>
       </c>
       <c r="C287">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.35">
@@ -3571,7 +3571,7 @@
         <v>3</v>
       </c>
       <c r="C288">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.35">
@@ -3582,7 +3582,7 @@
         <v>3</v>
       </c>
       <c r="C289">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.35">
@@ -3593,7 +3593,7 @@
         <v>3</v>
       </c>
       <c r="C290">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.35">
@@ -3604,7 +3604,7 @@
         <v>3</v>
       </c>
       <c r="C291">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.35">
@@ -3615,7 +3615,7 @@
         <v>3</v>
       </c>
       <c r="C292">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.35">
@@ -3626,7 +3626,7 @@
         <v>3</v>
       </c>
       <c r="C293">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.35">
@@ -3637,7 +3637,7 @@
         <v>3</v>
       </c>
       <c r="C294">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.35">
@@ -3648,7 +3648,7 @@
         <v>3</v>
       </c>
       <c r="C295">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.35">
@@ -3659,7 +3659,7 @@
         <v>3</v>
       </c>
       <c r="C296">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.35">
@@ -3670,7 +3670,7 @@
         <v>3</v>
       </c>
       <c r="C297">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.35">
@@ -3681,7 +3681,7 @@
         <v>3</v>
       </c>
       <c r="C298">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.35">
@@ -3692,7 +3692,7 @@
         <v>3</v>
       </c>
       <c r="C299">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.35">
@@ -3703,7 +3703,7 @@
         <v>3</v>
       </c>
       <c r="C300">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.35">
@@ -3714,7 +3714,7 @@
         <v>3</v>
       </c>
       <c r="C301">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.35">
@@ -3725,7 +3725,7 @@
         <v>3</v>
       </c>
       <c r="C302">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.35">
@@ -3736,7 +3736,7 @@
         <v>3</v>
       </c>
       <c r="C303">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.35">
@@ -3747,7 +3747,7 @@
         <v>3</v>
       </c>
       <c r="C304">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.35">
@@ -3758,7 +3758,7 @@
         <v>3</v>
       </c>
       <c r="C305">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.35">
@@ -3769,7 +3769,7 @@
         <v>3</v>
       </c>
       <c r="C306">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.35">
@@ -3780,7 +3780,7 @@
         <v>3</v>
       </c>
       <c r="C307">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.35">
@@ -3791,7 +3791,7 @@
         <v>3</v>
       </c>
       <c r="C308">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.35">
@@ -3802,7 +3802,7 @@
         <v>3</v>
       </c>
       <c r="C309">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.35">
@@ -3813,7 +3813,7 @@
         <v>3</v>
       </c>
       <c r="C310">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.35">
@@ -3824,7 +3824,7 @@
         <v>3</v>
       </c>
       <c r="C311">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.35">
@@ -3835,7 +3835,7 @@
         <v>3</v>
       </c>
       <c r="C312">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.35">
@@ -3846,7 +3846,7 @@
         <v>3</v>
       </c>
       <c r="C313">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.35">
@@ -3857,7 +3857,7 @@
         <v>3</v>
       </c>
       <c r="C314">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.35">
@@ -3868,7 +3868,7 @@
         <v>3</v>
       </c>
       <c r="C315">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.35">
@@ -3879,7 +3879,7 @@
         <v>3</v>
       </c>
       <c r="C316">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.35">
@@ -3890,7 +3890,7 @@
         <v>3</v>
       </c>
       <c r="C317">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.35">
@@ -3901,7 +3901,7 @@
         <v>3</v>
       </c>
       <c r="C318">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.35">
@@ -3912,7 +3912,7 @@
         <v>3</v>
       </c>
       <c r="C319">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.35">
@@ -3923,7 +3923,7 @@
         <v>3</v>
       </c>
       <c r="C320">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.35">
@@ -3934,7 +3934,7 @@
         <v>3</v>
       </c>
       <c r="C321">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.35">
@@ -3945,7 +3945,7 @@
         <v>3</v>
       </c>
       <c r="C322">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.35">
@@ -3956,7 +3956,7 @@
         <v>3</v>
       </c>
       <c r="C323">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.35">
@@ -3967,7 +3967,7 @@
         <v>3</v>
       </c>
       <c r="C324">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.35">
@@ -3978,7 +3978,7 @@
         <v>3</v>
       </c>
       <c r="C325">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.35">
@@ -3989,7 +3989,7 @@
         <v>3</v>
       </c>
       <c r="C326">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.35">
@@ -4000,7 +4000,7 @@
         <v>3</v>
       </c>
       <c r="C327">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.35">
@@ -4011,7 +4011,7 @@
         <v>3</v>
       </c>
       <c r="C328">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.35">
@@ -4022,7 +4022,7 @@
         <v>3</v>
       </c>
       <c r="C329">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.35">
@@ -4033,7 +4033,7 @@
         <v>3</v>
       </c>
       <c r="C330">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.35">
@@ -4044,7 +4044,7 @@
         <v>3</v>
       </c>
       <c r="C331">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.35">
@@ -4055,7 +4055,7 @@
         <v>3</v>
       </c>
       <c r="C332">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.35">
@@ -4066,7 +4066,7 @@
         <v>3</v>
       </c>
       <c r="C333">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.35">
@@ -4077,7 +4077,7 @@
         <v>3</v>
       </c>
       <c r="C334">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.35">
@@ -4088,7 +4088,7 @@
         <v>3</v>
       </c>
       <c r="C335">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.35">
@@ -4099,7 +4099,7 @@
         <v>3</v>
       </c>
       <c r="C336">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.35">
@@ -4110,7 +4110,7 @@
         <v>3</v>
       </c>
       <c r="C337">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.35">
@@ -4121,7 +4121,7 @@
         <v>3</v>
       </c>
       <c r="C338">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.35">
@@ -4132,7 +4132,7 @@
         <v>3</v>
       </c>
       <c r="C339">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.35">
@@ -4143,7 +4143,7 @@
         <v>3</v>
       </c>
       <c r="C340">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.35">
@@ -4154,7 +4154,7 @@
         <v>3</v>
       </c>
       <c r="C341">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.35">
@@ -4165,7 +4165,7 @@
         <v>3</v>
       </c>
       <c r="C342">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.35">
@@ -4176,7 +4176,7 @@
         <v>3</v>
       </c>
       <c r="C343">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.35">
@@ -4187,7 +4187,7 @@
         <v>3</v>
       </c>
       <c r="C344">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.35">
@@ -4198,7 +4198,7 @@
         <v>3</v>
       </c>
       <c r="C345">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.35">
@@ -4209,7 +4209,7 @@
         <v>3</v>
       </c>
       <c r="C346">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.35">
@@ -4220,7 +4220,7 @@
         <v>3</v>
       </c>
       <c r="C347">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.35">
@@ -4231,7 +4231,7 @@
         <v>3</v>
       </c>
       <c r="C348">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.35">
@@ -4242,7 +4242,7 @@
         <v>3</v>
       </c>
       <c r="C349">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.35">
@@ -4253,7 +4253,7 @@
         <v>3</v>
       </c>
       <c r="C350">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.35">
@@ -4264,7 +4264,7 @@
         <v>3</v>
       </c>
       <c r="C351">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.35">
@@ -4275,7 +4275,7 @@
         <v>3</v>
       </c>
       <c r="C352">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.35">
@@ -4286,7 +4286,7 @@
         <v>3</v>
       </c>
       <c r="C353">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.35">
@@ -4297,7 +4297,7 @@
         <v>3</v>
       </c>
       <c r="C354">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.35">
@@ -4308,7 +4308,7 @@
         <v>3</v>
       </c>
       <c r="C355">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.35">
@@ -4319,7 +4319,7 @@
         <v>3</v>
       </c>
       <c r="C356">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.35">
@@ -4330,7 +4330,7 @@
         <v>3</v>
       </c>
       <c r="C357">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.35">
@@ -4341,7 +4341,7 @@
         <v>3</v>
       </c>
       <c r="C358">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.35">
@@ -4352,7 +4352,7 @@
         <v>3</v>
       </c>
       <c r="C359">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.35">
@@ -4363,7 +4363,7 @@
         <v>3</v>
       </c>
       <c r="C360">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.35">
@@ -4374,7 +4374,7 @@
         <v>3</v>
       </c>
       <c r="C361">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.35">
@@ -4385,7 +4385,7 @@
         <v>3</v>
       </c>
       <c r="C362">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.35">
@@ -4396,7 +4396,7 @@
         <v>3</v>
       </c>
       <c r="C363">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.35">
@@ -4407,7 +4407,7 @@
         <v>3</v>
       </c>
       <c r="C364">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.35">
@@ -4418,7 +4418,7 @@
         <v>3</v>
       </c>
       <c r="C365">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.35">
@@ -4429,7 +4429,7 @@
         <v>3</v>
       </c>
       <c r="C366">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.35">
@@ -4440,7 +4440,7 @@
         <v>3</v>
       </c>
       <c r="C367">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.35">
@@ -4451,7 +4451,7 @@
         <v>3</v>
       </c>
       <c r="C368">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.35">
@@ -4462,7 +4462,7 @@
         <v>3</v>
       </c>
       <c r="C369">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.35">
@@ -4473,7 +4473,7 @@
         <v>3</v>
       </c>
       <c r="C370">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.35">
@@ -4484,7 +4484,7 @@
         <v>3</v>
       </c>
       <c r="C371">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.35">
@@ -4495,7 +4495,7 @@
         <v>3</v>
       </c>
       <c r="C372">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.35">
@@ -4506,7 +4506,7 @@
         <v>3</v>
       </c>
       <c r="C373">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.35">
@@ -4517,7 +4517,7 @@
         <v>3</v>
       </c>
       <c r="C374">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.35">
@@ -4528,7 +4528,7 @@
         <v>3</v>
       </c>
       <c r="C375">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.35">
@@ -4539,7 +4539,7 @@
         <v>3</v>
       </c>
       <c r="C376">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.35">
@@ -4550,7 +4550,7 @@
         <v>3</v>
       </c>
       <c r="C377">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.35">
@@ -4561,7 +4561,7 @@
         <v>3</v>
       </c>
       <c r="C378">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.35">
@@ -4572,7 +4572,7 @@
         <v>3</v>
       </c>
       <c r="C379">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.35">
@@ -4583,7 +4583,7 @@
         <v>3</v>
       </c>
       <c r="C380">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.35">
@@ -4594,7 +4594,7 @@
         <v>3</v>
       </c>
       <c r="C381">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.35">
@@ -4605,7 +4605,7 @@
         <v>3</v>
       </c>
       <c r="C382">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.35">
@@ -4616,7 +4616,7 @@
         <v>3</v>
       </c>
       <c r="C383">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.35">
@@ -4627,7 +4627,7 @@
         <v>3</v>
       </c>
       <c r="C384">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.35">
@@ -4638,7 +4638,7 @@
         <v>3</v>
       </c>
       <c r="C385">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.35">
@@ -4649,7 +4649,7 @@
         <v>3</v>
       </c>
       <c r="C386">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.35">
@@ -4660,7 +4660,7 @@
         <v>3</v>
       </c>
       <c r="C387">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.35">
@@ -4671,7 +4671,7 @@
         <v>3</v>
       </c>
       <c r="C388">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.35">
@@ -4682,7 +4682,7 @@
         <v>3</v>
       </c>
       <c r="C389">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.35">
@@ -4693,7 +4693,7 @@
         <v>3</v>
       </c>
       <c r="C390">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.35">
@@ -4704,7 +4704,7 @@
         <v>3</v>
       </c>
       <c r="C391">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.35">
@@ -4715,7 +4715,7 @@
         <v>3</v>
       </c>
       <c r="C392">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.35">
@@ -4726,7 +4726,7 @@
         <v>3</v>
       </c>
       <c r="C393">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.35">
@@ -4737,7 +4737,7 @@
         <v>3</v>
       </c>
       <c r="C394">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.35">
@@ -4748,7 +4748,7 @@
         <v>3</v>
       </c>
       <c r="C395">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.35">
@@ -4759,7 +4759,7 @@
         <v>3</v>
       </c>
       <c r="C396">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.35">
@@ -4770,7 +4770,7 @@
         <v>3</v>
       </c>
       <c r="C397">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.35">
@@ -4781,7 +4781,7 @@
         <v>3</v>
       </c>
       <c r="C398">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.35">
@@ -4792,7 +4792,7 @@
         <v>3</v>
       </c>
       <c r="C399">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.35">
@@ -4803,7 +4803,7 @@
         <v>3</v>
       </c>
       <c r="C400">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.35">
@@ -4814,7 +4814,7 @@
         <v>3</v>
       </c>
       <c r="C401">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.35">
@@ -4825,7 +4825,7 @@
         <v>3</v>
       </c>
       <c r="C402">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>